<commit_message>
chore: enhance test by add preprocess_text when find in each trie
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4364" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4374" uniqueCount="1140">
   <si>
     <t>Correct</t>
   </si>
@@ -3817,16 +3817,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>864</v>
+        <v>869</v>
       </c>
       <c r="B2">
         <v>1350</v>
       </c>
       <c r="C2">
-        <v>6.4</v>
+        <v>6.44</v>
       </c>
       <c r="D2">
-        <v>0.0001</v>
+        <v>0.0002</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -3954,7 +3954,7 @@
         <v>1</v>
       </c>
       <c r="S2">
-        <v>6.550000000000001E-05</v>
+        <v>0.000211542</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3995,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>2.2292E-05</v>
+        <v>7.083400000000001E-05</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -4048,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="S4">
-        <v>2.6917E-05</v>
+        <v>9.775E-05</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -4101,7 +4101,7 @@
         <v>1</v>
       </c>
       <c r="S5">
-        <v>3.0083E-05</v>
+        <v>9.854200000000001E-05</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -4154,7 +4154,7 @@
         <v>1</v>
       </c>
       <c r="S6">
-        <v>2.4542E-05</v>
+        <v>6.9125E-05</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -4213,7 +4213,7 @@
         <v>3</v>
       </c>
       <c r="S7">
-        <v>2.0042E-05</v>
+        <v>4.6083E-05</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -4272,7 +4272,7 @@
         <v>2</v>
       </c>
       <c r="S8">
-        <v>1.4875E-05</v>
+        <v>3.7042E-05</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -4331,7 +4331,7 @@
         <v>3</v>
       </c>
       <c r="S9">
-        <v>1.5959E-05</v>
+        <v>4.3041E-05</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -4390,7 +4390,7 @@
         <v>3</v>
       </c>
       <c r="S10">
-        <v>1.8833E-05</v>
+        <v>4.7625E-05</v>
       </c>
     </row>
     <row r="11" spans="1:19">
@@ -4449,7 +4449,7 @@
         <v>3</v>
       </c>
       <c r="S11">
-        <v>1.8917E-05</v>
+        <v>5.9459E-05</v>
       </c>
     </row>
     <row r="12" spans="1:19">
@@ -4496,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="S12">
-        <v>2.1542E-05</v>
+        <v>6.2166E-05</v>
       </c>
     </row>
     <row r="13" spans="1:19">
@@ -4555,7 +4555,7 @@
         <v>3</v>
       </c>
       <c r="S13">
-        <v>2.7666E-05</v>
+        <v>6.675E-05</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -4614,7 +4614,7 @@
         <v>3</v>
       </c>
       <c r="S14">
-        <v>2.7E-05</v>
+        <v>7.758300000000001E-05</v>
       </c>
     </row>
     <row r="15" spans="1:19">
@@ -4673,7 +4673,7 @@
         <v>3</v>
       </c>
       <c r="S15">
-        <v>2.9542E-05</v>
+        <v>9.125E-05</v>
       </c>
     </row>
     <row r="16" spans="1:19">
@@ -4732,7 +4732,7 @@
         <v>3</v>
       </c>
       <c r="S16">
-        <v>1.7625E-05</v>
+        <v>5.4708E-05</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -4791,7 +4791,7 @@
         <v>3</v>
       </c>
       <c r="S17">
-        <v>2.1041E-05</v>
+        <v>4.7625E-05</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -4850,7 +4850,7 @@
         <v>3</v>
       </c>
       <c r="S18">
-        <v>2.2E-05</v>
+        <v>4.7958E-05</v>
       </c>
     </row>
     <row r="19" spans="1:19">
@@ -4909,7 +4909,7 @@
         <v>3</v>
       </c>
       <c r="S19">
-        <v>1.725E-05</v>
+        <v>5.7875E-05</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -4968,7 +4968,7 @@
         <v>3</v>
       </c>
       <c r="S20">
-        <v>1.9834E-05</v>
+        <v>5.5916E-05</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -5027,7 +5027,7 @@
         <v>3</v>
       </c>
       <c r="S21">
-        <v>2.025E-05</v>
+        <v>4.5834E-05</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -5086,7 +5086,7 @@
         <v>3</v>
       </c>
       <c r="S22">
-        <v>2.5709E-05</v>
+        <v>6.904199999999999E-05</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -5145,7 +5145,7 @@
         <v>2</v>
       </c>
       <c r="S23">
-        <v>2.3125E-05</v>
+        <v>5E-05</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -5204,7 +5204,7 @@
         <v>3</v>
       </c>
       <c r="S24">
-        <v>1.8334E-05</v>
+        <v>4.6667E-05</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -5257,7 +5257,7 @@
         <v>2</v>
       </c>
       <c r="S25">
-        <v>1.7834E-05</v>
+        <v>4.8875E-05</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -5316,7 +5316,7 @@
         <v>3</v>
       </c>
       <c r="S26">
-        <v>1.6583E-05</v>
+        <v>3.8083E-05</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -5375,7 +5375,7 @@
         <v>3</v>
       </c>
       <c r="S27">
-        <v>2.2708E-05</v>
+        <v>3.725E-05</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -5434,7 +5434,7 @@
         <v>3</v>
       </c>
       <c r="S28">
-        <v>1.4084E-05</v>
+        <v>3.8833E-05</v>
       </c>
     </row>
     <row r="29" spans="1:19">
@@ -5493,7 +5493,7 @@
         <v>3</v>
       </c>
       <c r="S29">
-        <v>1.3417E-05</v>
+        <v>2.7625E-05</v>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -5534,7 +5534,7 @@
         <v>0</v>
       </c>
       <c r="S30">
-        <v>2.1083E-05</v>
+        <v>4.1458E-05</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -5593,7 +5593,7 @@
         <v>3</v>
       </c>
       <c r="S31">
-        <v>1.475E-05</v>
+        <v>2.4708E-05</v>
       </c>
     </row>
     <row r="32" spans="1:19">
@@ -5652,7 +5652,7 @@
         <v>3</v>
       </c>
       <c r="S32">
-        <v>1.9208E-05</v>
+        <v>4.0167E-05</v>
       </c>
     </row>
     <row r="33" spans="1:19">
@@ -5711,7 +5711,7 @@
         <v>3</v>
       </c>
       <c r="S33">
-        <v>1.55E-05</v>
+        <v>3.9833E-05</v>
       </c>
     </row>
     <row r="34" spans="1:19">
@@ -5770,7 +5770,7 @@
         <v>3</v>
       </c>
       <c r="S34">
-        <v>1.825E-05</v>
+        <v>5.8958E-05</v>
       </c>
     </row>
     <row r="35" spans="1:19">
@@ -5823,7 +5823,7 @@
         <v>2</v>
       </c>
       <c r="S35">
-        <v>2.0167E-05</v>
+        <v>4.775E-05</v>
       </c>
     </row>
     <row r="36" spans="1:19">
@@ -5876,7 +5876,7 @@
         <v>2</v>
       </c>
       <c r="S36">
-        <v>1.8333E-05</v>
+        <v>3.8625E-05</v>
       </c>
     </row>
     <row r="37" spans="1:19">
@@ -5935,7 +5935,7 @@
         <v>3</v>
       </c>
       <c r="S37">
-        <v>2.3334E-05</v>
+        <v>5.3292E-05</v>
       </c>
     </row>
     <row r="38" spans="1:19">
@@ -5994,7 +5994,7 @@
         <v>3</v>
       </c>
       <c r="S38">
-        <v>2.1334E-05</v>
+        <v>3.7375E-05</v>
       </c>
     </row>
     <row r="39" spans="1:19">
@@ -6053,7 +6053,7 @@
         <v>3</v>
       </c>
       <c r="S39">
-        <v>2.075E-05</v>
+        <v>3.375E-05</v>
       </c>
     </row>
     <row r="40" spans="1:19">
@@ -6106,7 +6106,7 @@
         <v>1</v>
       </c>
       <c r="S40">
-        <v>1.0375E-05</v>
+        <v>1.9625E-05</v>
       </c>
     </row>
     <row r="41" spans="1:19">
@@ -6165,7 +6165,7 @@
         <v>3</v>
       </c>
       <c r="S41">
-        <v>2.5583E-05</v>
+        <v>6.6209E-05</v>
       </c>
     </row>
     <row r="42" spans="1:19">
@@ -6224,7 +6224,7 @@
         <v>3</v>
       </c>
       <c r="S42">
-        <v>2.1375E-05</v>
+        <v>3.4917E-05</v>
       </c>
     </row>
     <row r="43" spans="1:19">
@@ -6283,7 +6283,7 @@
         <v>2</v>
       </c>
       <c r="S43">
-        <v>1.275E-05</v>
+        <v>2.1916E-05</v>
       </c>
     </row>
     <row r="44" spans="1:19">
@@ -6336,7 +6336,7 @@
         <v>2</v>
       </c>
       <c r="S44">
-        <v>1.9542E-05</v>
+        <v>3.9458E-05</v>
       </c>
     </row>
     <row r="45" spans="1:19">
@@ -6365,7 +6365,7 @@
         <v>2</v>
       </c>
       <c r="S45">
-        <v>1.45E-05</v>
+        <v>2.9458E-05</v>
       </c>
     </row>
     <row r="46" spans="1:19">
@@ -6424,7 +6424,7 @@
         <v>3</v>
       </c>
       <c r="S46">
-        <v>1.4041E-05</v>
+        <v>1.5958E-05</v>
       </c>
     </row>
     <row r="47" spans="1:19">
@@ -6483,7 +6483,7 @@
         <v>3</v>
       </c>
       <c r="S47">
-        <v>2.0167E-05</v>
+        <v>2.85E-05</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -6542,7 +6542,7 @@
         <v>3</v>
       </c>
       <c r="S48">
-        <v>1.675E-05</v>
+        <v>2.6375E-05</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -6601,7 +6601,7 @@
         <v>3</v>
       </c>
       <c r="S49">
-        <v>1.9959E-05</v>
+        <v>3.3959E-05</v>
       </c>
     </row>
     <row r="50" spans="1:19">
@@ -6654,7 +6654,7 @@
         <v>2</v>
       </c>
       <c r="S50">
-        <v>1.4458E-05</v>
+        <v>2.4333E-05</v>
       </c>
     </row>
     <row r="51" spans="1:19">
@@ -6713,7 +6713,7 @@
         <v>3</v>
       </c>
       <c r="S51">
-        <v>1.6125E-05</v>
+        <v>3.8334E-05</v>
       </c>
     </row>
     <row r="52" spans="1:19">
@@ -6766,7 +6766,7 @@
         <v>2</v>
       </c>
       <c r="S52">
-        <v>1.85E-05</v>
+        <v>3.3083E-05</v>
       </c>
     </row>
     <row r="53" spans="1:19">
@@ -6813,7 +6813,7 @@
         <v>1</v>
       </c>
       <c r="S53">
-        <v>2.4417E-05</v>
+        <v>3.5583E-05</v>
       </c>
     </row>
     <row r="54" spans="1:19">
@@ -6866,7 +6866,7 @@
         <v>1</v>
       </c>
       <c r="S54">
-        <v>1.5667E-05</v>
+        <v>2.5958E-05</v>
       </c>
     </row>
     <row r="55" spans="1:19">
@@ -6919,7 +6919,7 @@
         <v>2</v>
       </c>
       <c r="S55">
-        <v>1.5333E-05</v>
+        <v>2.8125E-05</v>
       </c>
     </row>
     <row r="56" spans="1:19">
@@ -6978,7 +6978,7 @@
         <v>3</v>
       </c>
       <c r="S56">
-        <v>1.6625E-05</v>
+        <v>2.9958E-05</v>
       </c>
     </row>
     <row r="57" spans="1:19">
@@ -7037,7 +7037,7 @@
         <v>2</v>
       </c>
       <c r="S57">
-        <v>1.3375E-05</v>
+        <v>2.1E-05</v>
       </c>
     </row>
     <row r="58" spans="1:19">
@@ -7084,7 +7084,7 @@
         <v>1</v>
       </c>
       <c r="S58">
-        <v>2.0792E-05</v>
+        <v>2.8625E-05</v>
       </c>
     </row>
     <row r="59" spans="1:19">
@@ -7143,7 +7143,7 @@
         <v>3</v>
       </c>
       <c r="S59">
-        <v>1.675E-05</v>
+        <v>2.1542E-05</v>
       </c>
     </row>
     <row r="60" spans="1:19">
@@ -7202,7 +7202,7 @@
         <v>3</v>
       </c>
       <c r="S60">
-        <v>2.3583E-05</v>
+        <v>4.9459E-05</v>
       </c>
     </row>
     <row r="61" spans="1:19">
@@ -7261,7 +7261,7 @@
         <v>3</v>
       </c>
       <c r="S61">
-        <v>1.3709E-05</v>
+        <v>2.3458E-05</v>
       </c>
     </row>
     <row r="62" spans="1:19">
@@ -7320,7 +7320,7 @@
         <v>3</v>
       </c>
       <c r="S62">
-        <v>1.8792E-05</v>
+        <v>3.5167E-05</v>
       </c>
     </row>
     <row r="63" spans="1:19">
@@ -7367,7 +7367,7 @@
         <v>1</v>
       </c>
       <c r="S63">
-        <v>1.9417E-05</v>
+        <v>3.5875E-05</v>
       </c>
     </row>
     <row r="64" spans="1:19">
@@ -7426,7 +7426,7 @@
         <v>3</v>
       </c>
       <c r="S64">
-        <v>2.1125E-05</v>
+        <v>4.1042E-05</v>
       </c>
     </row>
     <row r="65" spans="1:19">
@@ -7485,7 +7485,7 @@
         <v>3</v>
       </c>
       <c r="S65">
-        <v>2.0959E-05</v>
+        <v>4.8708E-05</v>
       </c>
     </row>
     <row r="66" spans="1:19">
@@ -7538,7 +7538,7 @@
         <v>2</v>
       </c>
       <c r="S66">
-        <v>1.5083E-05</v>
+        <v>2.4625E-05</v>
       </c>
     </row>
     <row r="67" spans="1:19">
@@ -7597,7 +7597,7 @@
         <v>3</v>
       </c>
       <c r="S67">
-        <v>2.0292E-05</v>
+        <v>4.0083E-05</v>
       </c>
     </row>
     <row r="68" spans="1:19">
@@ -7656,7 +7656,7 @@
         <v>3</v>
       </c>
       <c r="S68">
-        <v>1.3208E-05</v>
+        <v>2.0167E-05</v>
       </c>
     </row>
     <row r="69" spans="1:19">
@@ -7715,7 +7715,7 @@
         <v>3</v>
       </c>
       <c r="S69">
-        <v>1.9166E-05</v>
+        <v>4.9334E-05</v>
       </c>
     </row>
     <row r="70" spans="1:19">
@@ -7762,7 +7762,7 @@
         <v>1</v>
       </c>
       <c r="S70">
-        <v>1.2959E-05</v>
+        <v>2.7E-05</v>
       </c>
     </row>
     <row r="71" spans="1:19">
@@ -7821,7 +7821,7 @@
         <v>2</v>
       </c>
       <c r="S71">
-        <v>2.225E-05</v>
+        <v>5.7917E-05</v>
       </c>
     </row>
     <row r="72" spans="1:19">
@@ -7880,7 +7880,7 @@
         <v>3</v>
       </c>
       <c r="S72">
-        <v>1.2375E-05</v>
+        <v>2.5792E-05</v>
       </c>
     </row>
     <row r="73" spans="1:19">
@@ -7939,7 +7939,7 @@
         <v>3</v>
       </c>
       <c r="S73">
-        <v>1.3208E-05</v>
+        <v>2.225E-05</v>
       </c>
     </row>
     <row r="74" spans="1:19">
@@ -7998,7 +7998,7 @@
         <v>3</v>
       </c>
       <c r="S74">
-        <v>1.2292E-05</v>
+        <v>2.2E-05</v>
       </c>
     </row>
     <row r="75" spans="1:19">
@@ -8057,7 +8057,7 @@
         <v>3</v>
       </c>
       <c r="S75">
-        <v>1.475E-05</v>
+        <v>2.2E-05</v>
       </c>
     </row>
     <row r="76" spans="1:19">
@@ -8116,7 +8116,7 @@
         <v>3</v>
       </c>
       <c r="S76">
-        <v>1.725E-05</v>
+        <v>4.9083E-05</v>
       </c>
     </row>
     <row r="77" spans="1:19">
@@ -8169,7 +8169,7 @@
         <v>2</v>
       </c>
       <c r="S77">
-        <v>1.7208E-05</v>
+        <v>3.35E-05</v>
       </c>
     </row>
     <row r="78" spans="1:19">
@@ -8222,7 +8222,7 @@
         <v>2</v>
       </c>
       <c r="S78">
-        <v>1.5416E-05</v>
+        <v>3.65E-05</v>
       </c>
     </row>
     <row r="79" spans="1:19">
@@ -8281,7 +8281,7 @@
         <v>3</v>
       </c>
       <c r="S79">
-        <v>1.2834E-05</v>
+        <v>3.0667E-05</v>
       </c>
     </row>
     <row r="80" spans="1:19">
@@ -8322,7 +8322,7 @@
         <v>2</v>
       </c>
       <c r="S80">
-        <v>2.3666E-05</v>
+        <v>6.7375E-05</v>
       </c>
     </row>
     <row r="81" spans="1:19">
@@ -8381,7 +8381,7 @@
         <v>3</v>
       </c>
       <c r="S81">
-        <v>1.7458E-05</v>
+        <v>4.5833E-05</v>
       </c>
     </row>
     <row r="82" spans="1:19">
@@ -8440,7 +8440,7 @@
         <v>3</v>
       </c>
       <c r="S82">
-        <v>1.6834E-05</v>
+        <v>2.6709E-05</v>
       </c>
     </row>
     <row r="83" spans="1:19">
@@ -8499,7 +8499,7 @@
         <v>3</v>
       </c>
       <c r="S83">
-        <v>1.1916E-05</v>
+        <v>3.1834E-05</v>
       </c>
     </row>
     <row r="84" spans="1:19">
@@ -8540,7 +8540,7 @@
         <v>0</v>
       </c>
       <c r="S84">
-        <v>1.9542E-05</v>
+        <v>4.2417E-05</v>
       </c>
     </row>
     <row r="85" spans="1:19">
@@ -8599,7 +8599,7 @@
         <v>3</v>
       </c>
       <c r="S85">
-        <v>1.4958E-05</v>
+        <v>2.8834E-05</v>
       </c>
     </row>
     <row r="86" spans="1:19">
@@ -8658,7 +8658,7 @@
         <v>3</v>
       </c>
       <c r="S86">
-        <v>2.1625E-05</v>
+        <v>5.2291E-05</v>
       </c>
     </row>
     <row r="87" spans="1:19">
@@ -8687,7 +8687,7 @@
         <v>2</v>
       </c>
       <c r="S87">
-        <v>1.9375E-05</v>
+        <v>4.2E-05</v>
       </c>
     </row>
     <row r="88" spans="1:19">
@@ -8746,7 +8746,7 @@
         <v>3</v>
       </c>
       <c r="S88">
-        <v>3.2417E-05</v>
+        <v>6.2792E-05</v>
       </c>
     </row>
     <row r="89" spans="1:19">
@@ -8805,7 +8805,7 @@
         <v>3</v>
       </c>
       <c r="S89">
-        <v>9.75E-06</v>
+        <v>2.0708E-05</v>
       </c>
     </row>
     <row r="90" spans="1:19">
@@ -8864,7 +8864,7 @@
         <v>3</v>
       </c>
       <c r="S90">
-        <v>1.85E-05</v>
+        <v>4.0834E-05</v>
       </c>
     </row>
     <row r="91" spans="1:19">
@@ -8917,7 +8917,7 @@
         <v>2</v>
       </c>
       <c r="S91">
-        <v>1.35E-05</v>
+        <v>1.9833E-05</v>
       </c>
     </row>
     <row r="92" spans="1:19">
@@ -8964,7 +8964,7 @@
         <v>1</v>
       </c>
       <c r="S92">
-        <v>1.4458E-05</v>
+        <v>2.8542E-05</v>
       </c>
     </row>
     <row r="93" spans="1:19">
@@ -9023,7 +9023,7 @@
         <v>3</v>
       </c>
       <c r="S93">
-        <v>1.0709E-05</v>
+        <v>1.775E-05</v>
       </c>
     </row>
     <row r="94" spans="1:19">
@@ -9082,7 +9082,7 @@
         <v>3</v>
       </c>
       <c r="S94">
-        <v>7.417E-06</v>
+        <v>9.75E-06</v>
       </c>
     </row>
     <row r="95" spans="1:19">
@@ -9141,7 +9141,7 @@
         <v>2</v>
       </c>
       <c r="S95">
-        <v>1.6167E-05</v>
+        <v>3.3208E-05</v>
       </c>
     </row>
     <row r="96" spans="1:19">
@@ -9200,7 +9200,7 @@
         <v>3</v>
       </c>
       <c r="S96">
-        <v>1.35E-05</v>
+        <v>2.2584E-05</v>
       </c>
     </row>
     <row r="97" spans="1:19">
@@ -9259,7 +9259,7 @@
         <v>3</v>
       </c>
       <c r="S97">
-        <v>2.2083E-05</v>
+        <v>3.1959E-05</v>
       </c>
     </row>
     <row r="98" spans="1:19">
@@ -9318,7 +9318,7 @@
         <v>3</v>
       </c>
       <c r="S98">
-        <v>9.458E-06</v>
+        <v>1.1167E-05</v>
       </c>
     </row>
     <row r="99" spans="1:19">
@@ -9377,7 +9377,7 @@
         <v>3</v>
       </c>
       <c r="S99">
-        <v>9.833000000000001E-06</v>
+        <v>1.6125E-05</v>
       </c>
     </row>
     <row r="100" spans="1:19">
@@ -9436,7 +9436,7 @@
         <v>3</v>
       </c>
       <c r="S100">
-        <v>1.15E-05</v>
+        <v>2.575E-05</v>
       </c>
     </row>
     <row r="101" spans="1:19">
@@ -9489,7 +9489,7 @@
         <v>2</v>
       </c>
       <c r="S101">
-        <v>2E-05</v>
+        <v>3.0583E-05</v>
       </c>
     </row>
     <row r="102" spans="1:19">
@@ -9548,7 +9548,7 @@
         <v>2</v>
       </c>
       <c r="S102">
-        <v>1.4791E-05</v>
+        <v>2.9334E-05</v>
       </c>
     </row>
     <row r="103" spans="1:19">
@@ -9595,7 +9595,7 @@
         <v>1</v>
       </c>
       <c r="S103">
-        <v>1.9167E-05</v>
+        <v>2.0417E-05</v>
       </c>
     </row>
     <row r="104" spans="1:19">
@@ -9654,7 +9654,7 @@
         <v>3</v>
       </c>
       <c r="S104">
-        <v>2.1E-05</v>
+        <v>2.65E-05</v>
       </c>
     </row>
     <row r="105" spans="1:19">
@@ -9713,7 +9713,7 @@
         <v>3</v>
       </c>
       <c r="S105">
-        <v>1.7291E-05</v>
+        <v>2.1458E-05</v>
       </c>
     </row>
     <row r="106" spans="1:19">
@@ -9772,7 +9772,7 @@
         <v>3</v>
       </c>
       <c r="S106">
-        <v>1.4375E-05</v>
+        <v>3.025E-05</v>
       </c>
     </row>
     <row r="107" spans="1:19">
@@ -9831,7 +9831,7 @@
         <v>3</v>
       </c>
       <c r="S107">
-        <v>1.2042E-05</v>
+        <v>1.7792E-05</v>
       </c>
     </row>
     <row r="108" spans="1:19">
@@ -9890,7 +9890,7 @@
         <v>2</v>
       </c>
       <c r="S108">
-        <v>2.0666E-05</v>
+        <v>2.1584E-05</v>
       </c>
     </row>
     <row r="109" spans="1:19">
@@ -9949,7 +9949,7 @@
         <v>3</v>
       </c>
       <c r="S109">
-        <v>8.834E-06</v>
+        <v>1.7125E-05</v>
       </c>
     </row>
     <row r="110" spans="1:19">
@@ -9972,7 +9972,7 @@
         <v>3</v>
       </c>
       <c r="S110">
-        <v>1.9541E-05</v>
+        <v>5.4166E-05</v>
       </c>
     </row>
     <row r="111" spans="1:19">
@@ -10031,7 +10031,7 @@
         <v>3</v>
       </c>
       <c r="S111">
-        <v>1.7375E-05</v>
+        <v>2.875E-05</v>
       </c>
     </row>
     <row r="112" spans="1:19">
@@ -10084,7 +10084,7 @@
         <v>2</v>
       </c>
       <c r="S112">
-        <v>1.625E-05</v>
+        <v>2.825E-05</v>
       </c>
     </row>
     <row r="113" spans="1:19">
@@ -10143,7 +10143,7 @@
         <v>3</v>
       </c>
       <c r="S113">
-        <v>1.2584E-05</v>
+        <v>2.2625E-05</v>
       </c>
     </row>
     <row r="114" spans="1:19">
@@ -10178,7 +10178,7 @@
         <v>1</v>
       </c>
       <c r="S114">
-        <v>1.1542E-05</v>
+        <v>1.5167E-05</v>
       </c>
     </row>
     <row r="115" spans="1:19">
@@ -10219,7 +10219,7 @@
         <v>2</v>
       </c>
       <c r="S115">
-        <v>1.9375E-05</v>
+        <v>4.5E-05</v>
       </c>
     </row>
     <row r="116" spans="1:19">
@@ -10278,7 +10278,7 @@
         <v>3</v>
       </c>
       <c r="S116">
-        <v>1.4542E-05</v>
+        <v>2.8208E-05</v>
       </c>
     </row>
     <row r="117" spans="1:19">
@@ -10337,7 +10337,7 @@
         <v>3</v>
       </c>
       <c r="S117">
-        <v>1.6166E-05</v>
+        <v>3.2875E-05</v>
       </c>
     </row>
     <row r="118" spans="1:19">
@@ -10396,7 +10396,7 @@
         <v>3</v>
       </c>
       <c r="S118">
-        <v>1.5458E-05</v>
+        <v>2.6042E-05</v>
       </c>
     </row>
     <row r="119" spans="1:19">
@@ -10455,7 +10455,7 @@
         <v>3</v>
       </c>
       <c r="S119">
-        <v>1.85E-05</v>
+        <v>2.4125E-05</v>
       </c>
     </row>
     <row r="120" spans="1:19">
@@ -10514,7 +10514,7 @@
         <v>3</v>
       </c>
       <c r="S120">
-        <v>1.1458E-05</v>
+        <v>2.475E-05</v>
       </c>
     </row>
     <row r="121" spans="1:19">
@@ -10573,7 +10573,7 @@
         <v>3</v>
       </c>
       <c r="S121">
-        <v>1.0959E-05</v>
+        <v>2.2917E-05</v>
       </c>
     </row>
     <row r="122" spans="1:19">
@@ -10626,7 +10626,7 @@
         <v>2</v>
       </c>
       <c r="S122">
-        <v>1.8625E-05</v>
+        <v>2.9792E-05</v>
       </c>
     </row>
     <row r="123" spans="1:19">
@@ -10685,7 +10685,7 @@
         <v>3</v>
       </c>
       <c r="S123">
-        <v>9.792E-06</v>
+        <v>1.1583E-05</v>
       </c>
     </row>
     <row r="124" spans="1:19">
@@ -10726,7 +10726,7 @@
         <v>0</v>
       </c>
       <c r="S124">
-        <v>2.6417E-05</v>
+        <v>7.25E-05</v>
       </c>
     </row>
     <row r="125" spans="1:19">
@@ -10785,7 +10785,7 @@
         <v>3</v>
       </c>
       <c r="S125">
-        <v>1.25E-05</v>
+        <v>1.725E-05</v>
       </c>
     </row>
     <row r="126" spans="1:19">
@@ -10844,7 +10844,7 @@
         <v>2</v>
       </c>
       <c r="S126">
-        <v>1.3042E-05</v>
+        <v>1.9542E-05</v>
       </c>
     </row>
     <row r="127" spans="1:19">
@@ -10903,7 +10903,7 @@
         <v>3</v>
       </c>
       <c r="S127">
-        <v>1.5416E-05</v>
+        <v>3.4E-05</v>
       </c>
     </row>
     <row r="128" spans="1:19">
@@ -10962,7 +10962,7 @@
         <v>3</v>
       </c>
       <c r="S128">
-        <v>9.958E-06</v>
+        <v>1.9458E-05</v>
       </c>
     </row>
     <row r="129" spans="1:19">
@@ -11021,7 +11021,7 @@
         <v>3</v>
       </c>
       <c r="S129">
-        <v>1.5916E-05</v>
+        <v>2.3583E-05</v>
       </c>
     </row>
     <row r="130" spans="1:19">
@@ -11074,7 +11074,7 @@
         <v>2</v>
       </c>
       <c r="S130">
-        <v>9.292E-06</v>
+        <v>9.500000000000001E-06</v>
       </c>
     </row>
     <row r="131" spans="1:19">
@@ -11121,7 +11121,7 @@
         <v>1</v>
       </c>
       <c r="S131">
-        <v>1.0458E-05</v>
+        <v>1.4667E-05</v>
       </c>
     </row>
     <row r="132" spans="1:19">
@@ -11174,7 +11174,7 @@
         <v>2</v>
       </c>
       <c r="S132">
-        <v>1.6916E-05</v>
+        <v>3.35E-05</v>
       </c>
     </row>
     <row r="133" spans="1:19">
@@ -11233,7 +11233,7 @@
         <v>3</v>
       </c>
       <c r="S133">
-        <v>1.4292E-05</v>
+        <v>2.9709E-05</v>
       </c>
     </row>
     <row r="134" spans="1:19">
@@ -11292,7 +11292,7 @@
         <v>3</v>
       </c>
       <c r="S134">
-        <v>2.9E-05</v>
+        <v>4.4375E-05</v>
       </c>
     </row>
     <row r="135" spans="1:19">
@@ -11351,7 +11351,7 @@
         <v>3</v>
       </c>
       <c r="S135">
-        <v>1.9125E-05</v>
+        <v>2.3041E-05</v>
       </c>
     </row>
     <row r="136" spans="1:19">
@@ -11410,7 +11410,7 @@
         <v>3</v>
       </c>
       <c r="S136">
-        <v>1.3667E-05</v>
+        <v>2.7333E-05</v>
       </c>
     </row>
     <row r="137" spans="1:19">
@@ -11463,7 +11463,7 @@
         <v>2</v>
       </c>
       <c r="S137">
-        <v>1.4166E-05</v>
+        <v>2.1791E-05</v>
       </c>
     </row>
     <row r="138" spans="1:19">
@@ -11522,7 +11522,7 @@
         <v>3</v>
       </c>
       <c r="S138">
-        <v>9E-06</v>
+        <v>1.1125E-05</v>
       </c>
     </row>
     <row r="139" spans="1:19">
@@ -11581,7 +11581,7 @@
         <v>3</v>
       </c>
       <c r="S139">
-        <v>1.8541E-05</v>
+        <v>4.8125E-05</v>
       </c>
     </row>
     <row r="140" spans="1:19">
@@ -11640,7 +11640,7 @@
         <v>3</v>
       </c>
       <c r="S140">
-        <v>1.675E-05</v>
+        <v>2.3584E-05</v>
       </c>
     </row>
     <row r="141" spans="1:19">
@@ -11675,7 +11675,7 @@
         <v>1</v>
       </c>
       <c r="S141">
-        <v>1.1583E-05</v>
+        <v>2.6583E-05</v>
       </c>
     </row>
     <row r="142" spans="1:19">
@@ -11734,7 +11734,7 @@
         <v>2</v>
       </c>
       <c r="S142">
-        <v>9.041E-06</v>
+        <v>2.0625E-05</v>
       </c>
     </row>
     <row r="143" spans="1:19">
@@ -11793,7 +11793,7 @@
         <v>3</v>
       </c>
       <c r="S143">
-        <v>1.7333E-05</v>
+        <v>1.8625E-05</v>
       </c>
     </row>
     <row r="144" spans="1:19">
@@ -11846,7 +11846,7 @@
         <v>2</v>
       </c>
       <c r="S144">
-        <v>2.0666E-05</v>
+        <v>3.775E-05</v>
       </c>
     </row>
     <row r="145" spans="1:19">
@@ -11905,7 +11905,7 @@
         <v>3</v>
       </c>
       <c r="S145">
-        <v>1.325E-05</v>
+        <v>2.0458E-05</v>
       </c>
     </row>
     <row r="146" spans="1:19">
@@ -11964,7 +11964,7 @@
         <v>3</v>
       </c>
       <c r="S146">
-        <v>1.6167E-05</v>
+        <v>4.7958E-05</v>
       </c>
     </row>
     <row r="147" spans="1:19">
@@ -12023,7 +12023,7 @@
         <v>3</v>
       </c>
       <c r="S147">
-        <v>1.1708E-05</v>
+        <v>1.8541E-05</v>
       </c>
     </row>
     <row r="148" spans="1:19">
@@ -12082,7 +12082,7 @@
         <v>3</v>
       </c>
       <c r="S148">
-        <v>1.8083E-05</v>
+        <v>9.1875E-05</v>
       </c>
     </row>
     <row r="149" spans="1:19">
@@ -12135,7 +12135,7 @@
         <v>2</v>
       </c>
       <c r="S149">
-        <v>1.5709E-05</v>
+        <v>4.4458E-05</v>
       </c>
     </row>
     <row r="150" spans="1:19">
@@ -12188,7 +12188,7 @@
         <v>2</v>
       </c>
       <c r="S150">
-        <v>1.4208E-05</v>
+        <v>0.00010975</v>
       </c>
     </row>
     <row r="151" spans="1:19">
@@ -12247,7 +12247,7 @@
         <v>2</v>
       </c>
       <c r="S151">
-        <v>1.4833E-05</v>
+        <v>3.65E-05</v>
       </c>
     </row>
     <row r="152" spans="1:19">
@@ -12288,7 +12288,7 @@
         <v>2</v>
       </c>
       <c r="S152">
-        <v>9.041E-06</v>
+        <v>1.6083E-05</v>
       </c>
     </row>
     <row r="153" spans="1:19">
@@ -12335,7 +12335,7 @@
         <v>1</v>
       </c>
       <c r="S153">
-        <v>1.6208E-05</v>
+        <v>0.000140041</v>
       </c>
     </row>
     <row r="154" spans="1:19">
@@ -12382,7 +12382,7 @@
         <v>3</v>
       </c>
       <c r="S154">
-        <v>5.375E-06</v>
+        <v>7.1542E-05</v>
       </c>
     </row>
     <row r="155" spans="1:19">
@@ -12435,7 +12435,7 @@
         <v>1</v>
       </c>
       <c r="S155">
-        <v>9.583E-06</v>
+        <v>2.0416E-05</v>
       </c>
     </row>
     <row r="156" spans="1:19">
@@ -12482,7 +12482,7 @@
         <v>3</v>
       </c>
       <c r="S156">
-        <v>6.125E-06</v>
+        <v>1.45E-05</v>
       </c>
     </row>
     <row r="157" spans="1:19">
@@ -12523,7 +12523,7 @@
         <v>2</v>
       </c>
       <c r="S157">
-        <v>1.5833E-05</v>
+        <v>2.8375E-05</v>
       </c>
     </row>
     <row r="158" spans="1:19">
@@ -12570,7 +12570,7 @@
         <v>3</v>
       </c>
       <c r="S158">
-        <v>8.167E-06</v>
+        <v>1.725E-05</v>
       </c>
     </row>
     <row r="159" spans="1:19">
@@ -12629,7 +12629,7 @@
         <v>2</v>
       </c>
       <c r="S159">
-        <v>8.667E-06</v>
+        <v>1.4541E-05</v>
       </c>
     </row>
     <row r="160" spans="1:19">
@@ -12676,7 +12676,7 @@
         <v>1</v>
       </c>
       <c r="S160">
-        <v>9.042000000000001E-06</v>
+        <v>1.4209E-05</v>
       </c>
     </row>
     <row r="161" spans="1:19">
@@ -12729,7 +12729,7 @@
         <v>2</v>
       </c>
       <c r="S161">
-        <v>1.3958E-05</v>
+        <v>3.1834E-05</v>
       </c>
     </row>
     <row r="162" spans="1:19">
@@ -12782,7 +12782,7 @@
         <v>2</v>
       </c>
       <c r="S162">
-        <v>1.2125E-05</v>
+        <v>2.5333E-05</v>
       </c>
     </row>
     <row r="163" spans="1:19">
@@ -12829,7 +12829,7 @@
         <v>1</v>
       </c>
       <c r="S163">
-        <v>2.175E-05</v>
+        <v>6.8042E-05</v>
       </c>
     </row>
     <row r="164" spans="1:19">
@@ -12888,7 +12888,7 @@
         <v>2</v>
       </c>
       <c r="S164">
-        <v>2.1834E-05</v>
+        <v>0.0001145</v>
       </c>
     </row>
     <row r="165" spans="1:19">
@@ -12947,7 +12947,7 @@
         <v>2</v>
       </c>
       <c r="S165">
-        <v>1.1667E-05</v>
+        <v>0.000203958</v>
       </c>
     </row>
     <row r="166" spans="1:19">
@@ -12994,7 +12994,7 @@
         <v>1</v>
       </c>
       <c r="S166">
-        <v>1.5208E-05</v>
+        <v>9.8625E-05</v>
       </c>
     </row>
     <row r="167" spans="1:19">
@@ -13041,7 +13041,7 @@
         <v>1</v>
       </c>
       <c r="S167">
-        <v>8.375E-06</v>
+        <v>9.1375E-05</v>
       </c>
     </row>
     <row r="168" spans="1:19">
@@ -13088,7 +13088,7 @@
         <v>3</v>
       </c>
       <c r="S168">
-        <v>9.667000000000001E-06</v>
+        <v>3.9958E-05</v>
       </c>
     </row>
     <row r="169" spans="1:19">
@@ -13129,7 +13129,7 @@
         <v>2</v>
       </c>
       <c r="S169">
-        <v>9E-06</v>
+        <v>2.2667E-05</v>
       </c>
     </row>
     <row r="170" spans="1:19">
@@ -13176,7 +13176,7 @@
         <v>1</v>
       </c>
       <c r="S170">
-        <v>8.250000000000001E-06</v>
+        <v>3.6542E-05</v>
       </c>
     </row>
     <row r="171" spans="1:19">
@@ -13217,7 +13217,7 @@
         <v>0</v>
       </c>
       <c r="S171">
-        <v>1.0667E-05</v>
+        <v>8.9417E-05</v>
       </c>
     </row>
     <row r="172" spans="1:19">
@@ -13264,7 +13264,7 @@
         <v>3</v>
       </c>
       <c r="S172">
-        <v>7.791999999999999E-06</v>
+        <v>4.425E-05</v>
       </c>
     </row>
     <row r="173" spans="1:19">
@@ -13311,7 +13311,7 @@
         <v>3</v>
       </c>
       <c r="S173">
-        <v>8.625E-06</v>
+        <v>3.3E-05</v>
       </c>
     </row>
     <row r="174" spans="1:19">
@@ -13358,7 +13358,7 @@
         <v>3</v>
       </c>
       <c r="S174">
-        <v>8.459E-06</v>
+        <v>0.000100083</v>
       </c>
     </row>
     <row r="175" spans="1:19">
@@ -13417,7 +13417,7 @@
         <v>1</v>
       </c>
       <c r="S175">
-        <v>1.2041E-05</v>
+        <v>7.6667E-05</v>
       </c>
     </row>
     <row r="176" spans="1:19">
@@ -13452,7 +13452,7 @@
         <v>1</v>
       </c>
       <c r="S176">
-        <v>6.166E-06</v>
+        <v>3.825E-05</v>
       </c>
     </row>
     <row r="177" spans="1:19">
@@ -13493,7 +13493,7 @@
         <v>2</v>
       </c>
       <c r="S177">
-        <v>7.084E-06</v>
+        <v>3.9667E-05</v>
       </c>
     </row>
     <row r="178" spans="1:19">
@@ -13546,7 +13546,7 @@
         <v>2</v>
       </c>
       <c r="S178">
-        <v>8.749999999999999E-06</v>
+        <v>9.8291E-05</v>
       </c>
     </row>
     <row r="179" spans="1:19">
@@ -13581,7 +13581,7 @@
         <v>1</v>
       </c>
       <c r="S179">
-        <v>6.25E-06</v>
+        <v>3.3166E-05</v>
       </c>
     </row>
     <row r="180" spans="1:19">
@@ -13622,7 +13622,7 @@
         <v>0</v>
       </c>
       <c r="S180">
-        <v>1.45E-05</v>
+        <v>0.000124584</v>
       </c>
     </row>
     <row r="181" spans="1:19">
@@ -13675,7 +13675,7 @@
         <v>1</v>
       </c>
       <c r="S181">
-        <v>7.875E-06</v>
+        <v>8.1541E-05</v>
       </c>
     </row>
     <row r="182" spans="1:19">
@@ -13722,7 +13722,7 @@
         <v>1</v>
       </c>
       <c r="S182">
-        <v>1.3042E-05</v>
+        <v>8.7292E-05</v>
       </c>
     </row>
     <row r="183" spans="1:19">
@@ -13769,7 +13769,7 @@
         <v>1</v>
       </c>
       <c r="S183">
-        <v>8.209000000000001E-06</v>
+        <v>3.3708E-05</v>
       </c>
     </row>
     <row r="184" spans="1:19">
@@ -13804,7 +13804,7 @@
         <v>1</v>
       </c>
       <c r="S184">
-        <v>6.292E-06</v>
+        <v>2.0875E-05</v>
       </c>
     </row>
     <row r="185" spans="1:19">
@@ -13851,7 +13851,7 @@
         <v>3</v>
       </c>
       <c r="S185">
-        <v>6.292E-06</v>
+        <v>3.2834E-05</v>
       </c>
     </row>
     <row r="186" spans="1:19">
@@ -13892,7 +13892,7 @@
         <v>1</v>
       </c>
       <c r="S186">
-        <v>1.0375E-05</v>
+        <v>1.8958E-05</v>
       </c>
     </row>
     <row r="187" spans="1:19">
@@ -13933,7 +13933,7 @@
         <v>0</v>
       </c>
       <c r="S187">
-        <v>1.65E-05</v>
+        <v>9.174999999999999E-05</v>
       </c>
     </row>
     <row r="188" spans="1:19">
@@ -13980,7 +13980,7 @@
         <v>3</v>
       </c>
       <c r="S188">
-        <v>6.334E-06</v>
+        <v>3.0291E-05</v>
       </c>
     </row>
     <row r="189" spans="1:19">
@@ -14015,7 +14015,7 @@
         <v>1</v>
       </c>
       <c r="S189">
-        <v>1.2125E-05</v>
+        <v>4.8291E-05</v>
       </c>
     </row>
     <row r="190" spans="1:19">
@@ -14068,7 +14068,7 @@
         <v>2</v>
       </c>
       <c r="S190">
-        <v>5.834E-06</v>
+        <v>9.25E-05</v>
       </c>
     </row>
     <row r="191" spans="1:19">
@@ -14121,7 +14121,7 @@
         <v>2</v>
       </c>
       <c r="S191">
-        <v>1.1625E-05</v>
+        <v>6.9792E-05</v>
       </c>
     </row>
     <row r="192" spans="1:19">
@@ -14168,7 +14168,7 @@
         <v>3</v>
       </c>
       <c r="S192">
-        <v>9.75E-06</v>
+        <v>4.3333E-05</v>
       </c>
     </row>
     <row r="193" spans="1:19">
@@ -14215,7 +14215,7 @@
         <v>1</v>
       </c>
       <c r="S193">
-        <v>9.583E-06</v>
+        <v>5.0334E-05</v>
       </c>
     </row>
     <row r="194" spans="1:19">
@@ -14274,7 +14274,7 @@
         <v>3</v>
       </c>
       <c r="S194">
-        <v>9.916E-06</v>
+        <v>7.404199999999999E-05</v>
       </c>
     </row>
     <row r="195" spans="1:19">
@@ -14315,7 +14315,7 @@
         <v>2</v>
       </c>
       <c r="S195">
-        <v>7.167E-06</v>
+        <v>4.5708E-05</v>
       </c>
     </row>
     <row r="196" spans="1:19">
@@ -14368,7 +14368,7 @@
         <v>2</v>
       </c>
       <c r="S196">
-        <v>9.292E-06</v>
+        <v>5.9709E-05</v>
       </c>
     </row>
     <row r="197" spans="1:19">
@@ -14403,7 +14403,7 @@
         <v>1</v>
       </c>
       <c r="S197">
-        <v>6E-06</v>
+        <v>2.7791E-05</v>
       </c>
     </row>
     <row r="198" spans="1:19">
@@ -14444,7 +14444,7 @@
         <v>2</v>
       </c>
       <c r="S198">
-        <v>6.333E-06</v>
+        <v>3.9792E-05</v>
       </c>
     </row>
     <row r="199" spans="1:19">
@@ -14491,7 +14491,7 @@
         <v>1</v>
       </c>
       <c r="S199">
-        <v>1.2334E-05</v>
+        <v>0.000102041</v>
       </c>
     </row>
     <row r="200" spans="1:19">
@@ -14532,7 +14532,7 @@
         <v>0</v>
       </c>
       <c r="S200">
-        <v>1.7875E-05</v>
+        <v>0.00011025</v>
       </c>
     </row>
     <row r="201" spans="1:19">
@@ -14585,7 +14585,7 @@
         <v>2</v>
       </c>
       <c r="S201">
-        <v>1.4208E-05</v>
+        <v>9.05E-05</v>
       </c>
     </row>
     <row r="202" spans="1:19">
@@ -14626,7 +14626,7 @@
         <v>2</v>
       </c>
       <c r="S202">
-        <v>8.833E-06</v>
+        <v>3.5375E-05</v>
       </c>
     </row>
     <row r="203" spans="1:19">
@@ -14661,7 +14661,7 @@
         <v>1</v>
       </c>
       <c r="S203">
-        <v>1.0292E-05</v>
+        <v>5.975E-05</v>
       </c>
     </row>
     <row r="204" spans="1:19">
@@ -14702,7 +14702,7 @@
         <v>0</v>
       </c>
       <c r="S204">
-        <v>2.4208E-05</v>
+        <v>7.741699999999999E-05</v>
       </c>
     </row>
     <row r="205" spans="1:19">
@@ -14755,7 +14755,7 @@
         <v>1</v>
       </c>
       <c r="S205">
-        <v>1.1958E-05</v>
+        <v>2.4792E-05</v>
       </c>
     </row>
     <row r="206" spans="1:19">
@@ -14790,7 +14790,7 @@
         <v>1</v>
       </c>
       <c r="S206">
-        <v>7.458E-06</v>
+        <v>1.9917E-05</v>
       </c>
     </row>
     <row r="207" spans="1:19">
@@ -14825,7 +14825,7 @@
         <v>1</v>
       </c>
       <c r="S207">
-        <v>7.416E-06</v>
+        <v>4.3209E-05</v>
       </c>
     </row>
     <row r="208" spans="1:19">
@@ -14838,11 +14838,17 @@
       <c r="C208" t="s">
         <v>484</v>
       </c>
+      <c r="D208" t="s">
+        <v>484</v>
+      </c>
       <c r="E208" t="s">
         <v>484</v>
       </c>
+      <c r="F208" t="s">
+        <v>484</v>
+      </c>
       <c r="G208">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H208" t="s">
         <v>673</v>
@@ -14863,10 +14869,10 @@
         <v>0</v>
       </c>
       <c r="R208">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S208">
-        <v>1.5E-05</v>
+        <v>9.4292E-05</v>
       </c>
     </row>
     <row r="209" spans="1:19">
@@ -14913,7 +14919,7 @@
         <v>3</v>
       </c>
       <c r="S209">
-        <v>9.792E-06</v>
+        <v>7.5208E-05</v>
       </c>
     </row>
     <row r="210" spans="1:19">
@@ -14948,7 +14954,7 @@
         <v>1</v>
       </c>
       <c r="S210">
-        <v>7.5E-06</v>
+        <v>5.6541E-05</v>
       </c>
     </row>
     <row r="211" spans="1:19">
@@ -14995,7 +15001,7 @@
         <v>2</v>
       </c>
       <c r="S211">
-        <v>7.125E-06</v>
+        <v>3.0125E-05</v>
       </c>
     </row>
     <row r="212" spans="1:19">
@@ -15042,7 +15048,7 @@
         <v>2</v>
       </c>
       <c r="S212">
-        <v>7.917000000000001E-06</v>
+        <v>4.9834E-05</v>
       </c>
     </row>
     <row r="213" spans="1:19">
@@ -15077,7 +15083,7 @@
         <v>1</v>
       </c>
       <c r="S213">
-        <v>1.3208E-05</v>
+        <v>7.4834E-05</v>
       </c>
     </row>
     <row r="214" spans="1:19">
@@ -15124,7 +15130,7 @@
         <v>3</v>
       </c>
       <c r="S214">
-        <v>7E-06</v>
+        <v>3.9333E-05</v>
       </c>
     </row>
     <row r="215" spans="1:19">
@@ -15171,7 +15177,7 @@
         <v>1</v>
       </c>
       <c r="S215">
-        <v>1.1541E-05</v>
+        <v>7.6209E-05</v>
       </c>
     </row>
     <row r="216" spans="1:19">
@@ -15212,7 +15218,7 @@
         <v>2</v>
       </c>
       <c r="S216">
-        <v>6.833E-06</v>
+        <v>4.1125E-05</v>
       </c>
     </row>
     <row r="217" spans="1:19">
@@ -15247,7 +15253,7 @@
         <v>1</v>
       </c>
       <c r="S217">
-        <v>8.334E-06</v>
+        <v>5.7208E-05</v>
       </c>
     </row>
     <row r="218" spans="1:19">
@@ -15288,7 +15294,7 @@
         <v>2</v>
       </c>
       <c r="S218">
-        <v>6.459E-06</v>
+        <v>4.4375E-05</v>
       </c>
     </row>
     <row r="219" spans="1:19">
@@ -15329,7 +15335,7 @@
         <v>2</v>
       </c>
       <c r="S219">
-        <v>4.333E-06</v>
+        <v>3.0709E-05</v>
       </c>
     </row>
     <row r="220" spans="1:19">
@@ -15370,7 +15376,7 @@
         <v>2</v>
       </c>
       <c r="S220">
-        <v>4.375E-06</v>
+        <v>2.15E-05</v>
       </c>
     </row>
     <row r="221" spans="1:19">
@@ -15423,7 +15429,7 @@
         <v>2</v>
       </c>
       <c r="S221">
-        <v>1.1125E-05</v>
+        <v>2.6542E-05</v>
       </c>
     </row>
     <row r="222" spans="1:19">
@@ -15476,7 +15482,7 @@
         <v>2</v>
       </c>
       <c r="S222">
-        <v>1.2333E-05</v>
+        <v>5.4417E-05</v>
       </c>
     </row>
     <row r="223" spans="1:19">
@@ -15535,7 +15541,7 @@
         <v>3</v>
       </c>
       <c r="S223">
-        <v>1.0875E-05</v>
+        <v>6.05E-05</v>
       </c>
     </row>
     <row r="224" spans="1:19">
@@ -15576,7 +15582,7 @@
         <v>2</v>
       </c>
       <c r="S224">
-        <v>9.084E-06</v>
+        <v>0.000124042</v>
       </c>
     </row>
     <row r="225" spans="1:19">
@@ -15617,7 +15623,7 @@
         <v>2</v>
       </c>
       <c r="S225">
-        <v>8.875000000000001E-06</v>
+        <v>6.0083E-05</v>
       </c>
     </row>
     <row r="226" spans="1:19">
@@ -15664,7 +15670,7 @@
         <v>1</v>
       </c>
       <c r="S226">
-        <v>1.2E-05</v>
+        <v>8.4125E-05</v>
       </c>
     </row>
     <row r="227" spans="1:19">
@@ -15711,7 +15717,7 @@
         <v>2</v>
       </c>
       <c r="S227">
-        <v>7.875E-06</v>
+        <v>4.9625E-05</v>
       </c>
     </row>
     <row r="228" spans="1:19">
@@ -15764,7 +15770,7 @@
         <v>1</v>
       </c>
       <c r="S228">
-        <v>2.0125E-05</v>
+        <v>0.000103667</v>
       </c>
     </row>
     <row r="229" spans="1:19">
@@ -15805,7 +15811,7 @@
         <v>0</v>
       </c>
       <c r="S229">
-        <v>1.7042E-05</v>
+        <v>4.9375E-05</v>
       </c>
     </row>
     <row r="230" spans="1:19">
@@ -15846,7 +15852,7 @@
         <v>0</v>
       </c>
       <c r="S230">
-        <v>1.8666E-05</v>
+        <v>5.3625E-05</v>
       </c>
     </row>
     <row r="231" spans="1:19">
@@ -15893,7 +15899,7 @@
         <v>1</v>
       </c>
       <c r="S231">
-        <v>1.7166E-05</v>
+        <v>4.5959E-05</v>
       </c>
     </row>
     <row r="232" spans="1:19">
@@ -15915,11 +15921,17 @@
       <c r="H232" t="s">
         <v>555</v>
       </c>
+      <c r="I232" t="s">
+        <v>555</v>
+      </c>
       <c r="J232" t="s">
         <v>555</v>
       </c>
+      <c r="K232" t="s">
+        <v>555</v>
+      </c>
       <c r="L232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M232" t="s">
         <v>973</v>
@@ -15931,10 +15943,10 @@
         <v>0</v>
       </c>
       <c r="R232">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S232">
-        <v>1.0375E-05</v>
+        <v>2.6083E-05</v>
       </c>
     </row>
     <row r="233" spans="1:19">
@@ -15975,7 +15987,7 @@
         <v>0</v>
       </c>
       <c r="S233">
-        <v>1.3875E-05</v>
+        <v>3.7208E-05</v>
       </c>
     </row>
     <row r="234" spans="1:19">
@@ -16016,7 +16028,7 @@
         <v>2</v>
       </c>
       <c r="S234">
-        <v>9.125E-06</v>
+        <v>3.5E-05</v>
       </c>
     </row>
     <row r="235" spans="1:19">
@@ -16063,7 +16075,7 @@
         <v>2</v>
       </c>
       <c r="S235">
-        <v>1.1375E-05</v>
+        <v>6.05E-05</v>
       </c>
     </row>
     <row r="236" spans="1:19">
@@ -16104,7 +16116,7 @@
         <v>2</v>
       </c>
       <c r="S236">
-        <v>1.3375E-05</v>
+        <v>6.7875E-05</v>
       </c>
     </row>
     <row r="237" spans="1:19">
@@ -16145,7 +16157,7 @@
         <v>2</v>
       </c>
       <c r="S237">
-        <v>6.917E-06</v>
+        <v>1.9541E-05</v>
       </c>
     </row>
     <row r="238" spans="1:19">
@@ -16198,7 +16210,7 @@
         <v>2</v>
       </c>
       <c r="S238">
-        <v>1.3041E-05</v>
+        <v>7.5584E-05</v>
       </c>
     </row>
     <row r="239" spans="1:19">
@@ -16233,7 +16245,7 @@
         <v>1</v>
       </c>
       <c r="S239">
-        <v>5.292E-06</v>
+        <v>1.8375E-05</v>
       </c>
     </row>
     <row r="240" spans="1:19">
@@ -16274,7 +16286,7 @@
         <v>2</v>
       </c>
       <c r="S240">
-        <v>8.542000000000001E-06</v>
+        <v>5.85E-05</v>
       </c>
     </row>
     <row r="241" spans="1:19">
@@ -16309,7 +16321,7 @@
         <v>1</v>
       </c>
       <c r="S241">
-        <v>1.1084E-05</v>
+        <v>4.7708E-05</v>
       </c>
     </row>
     <row r="242" spans="1:19">
@@ -16356,7 +16368,7 @@
         <v>1</v>
       </c>
       <c r="S242">
-        <v>2.4E-05</v>
+        <v>7.483300000000001E-05</v>
       </c>
     </row>
     <row r="243" spans="1:19">
@@ -16403,7 +16415,7 @@
         <v>3</v>
       </c>
       <c r="S243">
-        <v>5.417E-06</v>
+        <v>1.4625E-05</v>
       </c>
     </row>
     <row r="244" spans="1:19">
@@ -16450,7 +16462,7 @@
         <v>3</v>
       </c>
       <c r="S244">
-        <v>5.541E-06</v>
+        <v>1.0459E-05</v>
       </c>
     </row>
     <row r="245" spans="1:19">
@@ -16497,7 +16509,7 @@
         <v>1</v>
       </c>
       <c r="S245">
-        <v>1.1209E-05</v>
+        <v>2.2208E-05</v>
       </c>
     </row>
     <row r="246" spans="1:19">
@@ -16544,7 +16556,7 @@
         <v>2</v>
       </c>
       <c r="S246">
-        <v>1.3416E-05</v>
+        <v>1.8958E-05</v>
       </c>
     </row>
     <row r="247" spans="1:19">
@@ -16579,7 +16591,7 @@
         <v>1</v>
       </c>
       <c r="S247">
-        <v>6.5E-06</v>
+        <v>6.084E-06</v>
       </c>
     </row>
     <row r="248" spans="1:19">
@@ -16626,7 +16638,7 @@
         <v>1</v>
       </c>
       <c r="S248">
-        <v>1.2708E-05</v>
+        <v>3.0042E-05</v>
       </c>
     </row>
     <row r="249" spans="1:19">
@@ -16661,7 +16673,7 @@
         <v>1</v>
       </c>
       <c r="S249">
-        <v>3.916E-06</v>
+        <v>5.375E-06</v>
       </c>
     </row>
     <row r="250" spans="1:19">
@@ -16714,7 +16726,7 @@
         <v>2</v>
       </c>
       <c r="S250">
-        <v>1.475E-05</v>
+        <v>4.125E-05</v>
       </c>
     </row>
     <row r="251" spans="1:19">
@@ -16761,7 +16773,7 @@
         <v>1</v>
       </c>
       <c r="S251">
-        <v>1.1625E-05</v>
+        <v>3.2375E-05</v>
       </c>
     </row>
     <row r="252" spans="1:19">
@@ -16802,7 +16814,7 @@
         <v>1</v>
       </c>
       <c r="S252">
-        <v>6.583E-06</v>
+        <v>1.05E-05</v>
       </c>
     </row>
     <row r="253" spans="1:19">
@@ -16843,7 +16855,7 @@
         <v>2</v>
       </c>
       <c r="S253">
-        <v>4.292E-06</v>
+        <v>9.167E-06</v>
       </c>
     </row>
     <row r="254" spans="1:19">
@@ -16890,7 +16902,7 @@
         <v>1</v>
       </c>
       <c r="S254">
-        <v>8.583000000000001E-06</v>
+        <v>1.4667E-05</v>
       </c>
     </row>
     <row r="255" spans="1:19">
@@ -16949,7 +16961,7 @@
         <v>2</v>
       </c>
       <c r="S255">
-        <v>7.417E-06</v>
+        <v>1.7292E-05</v>
       </c>
     </row>
     <row r="256" spans="1:19">
@@ -16996,7 +17008,7 @@
         <v>3</v>
       </c>
       <c r="S256">
-        <v>1.0917E-05</v>
+        <v>2.7625E-05</v>
       </c>
     </row>
     <row r="257" spans="1:19">
@@ -17055,7 +17067,7 @@
         <v>3</v>
       </c>
       <c r="S257">
-        <v>9.042000000000001E-06</v>
+        <v>1.3917E-05</v>
       </c>
     </row>
     <row r="258" spans="1:19">
@@ -17108,7 +17120,7 @@
         <v>1</v>
       </c>
       <c r="S258">
-        <v>1.3041E-05</v>
+        <v>2.625E-05</v>
       </c>
     </row>
     <row r="259" spans="1:19">
@@ -17149,7 +17161,7 @@
         <v>2</v>
       </c>
       <c r="S259">
-        <v>1.0542E-05</v>
+        <v>2.6958E-05</v>
       </c>
     </row>
     <row r="260" spans="1:19">
@@ -17184,7 +17196,7 @@
         <v>1</v>
       </c>
       <c r="S260">
-        <v>6.542E-06</v>
+        <v>1.2083E-05</v>
       </c>
     </row>
     <row r="261" spans="1:19">
@@ -17225,7 +17237,7 @@
         <v>2</v>
       </c>
       <c r="S261">
-        <v>7.625E-06</v>
+        <v>1.5042E-05</v>
       </c>
     </row>
     <row r="262" spans="1:19">
@@ -17266,7 +17278,7 @@
         <v>2</v>
       </c>
       <c r="S262">
-        <v>6.5E-06</v>
+        <v>9.707999999999999E-06</v>
       </c>
     </row>
     <row r="263" spans="1:19">
@@ -17307,7 +17319,7 @@
         <v>2</v>
       </c>
       <c r="S263">
-        <v>5.208E-06</v>
+        <v>9.082999999999999E-06</v>
       </c>
     </row>
     <row r="264" spans="1:19">
@@ -17354,7 +17366,7 @@
         <v>3</v>
       </c>
       <c r="S264">
-        <v>6.625E-06</v>
+        <v>1.1375E-05</v>
       </c>
     </row>
     <row r="265" spans="1:19">
@@ -17395,7 +17407,7 @@
         <v>2</v>
       </c>
       <c r="S265">
-        <v>1.0291E-05</v>
+        <v>1.4667E-05</v>
       </c>
     </row>
     <row r="266" spans="1:19">
@@ -17436,7 +17448,7 @@
         <v>2</v>
       </c>
       <c r="S266">
-        <v>9.75E-06</v>
+        <v>2.3875E-05</v>
       </c>
     </row>
     <row r="267" spans="1:19">
@@ -17477,7 +17489,7 @@
         <v>2</v>
       </c>
       <c r="S267">
-        <v>7.75E-06</v>
+        <v>1.9125E-05</v>
       </c>
     </row>
     <row r="268" spans="1:19">
@@ -17530,7 +17542,7 @@
         <v>2</v>
       </c>
       <c r="S268">
-        <v>1.175E-05</v>
+        <v>2.8666E-05</v>
       </c>
     </row>
     <row r="269" spans="1:19">
@@ -17577,7 +17589,7 @@
         <v>1</v>
       </c>
       <c r="S269">
-        <v>1.6792E-05</v>
+        <v>4.1541E-05</v>
       </c>
     </row>
     <row r="270" spans="1:19">
@@ -17624,7 +17636,7 @@
         <v>2</v>
       </c>
       <c r="S270">
-        <v>8.416999999999999E-06</v>
+        <v>7.334E-06</v>
       </c>
     </row>
     <row r="271" spans="1:19">
@@ -17671,7 +17683,7 @@
         <v>1</v>
       </c>
       <c r="S271">
-        <v>1.5958E-05</v>
+        <v>3.5333E-05</v>
       </c>
     </row>
     <row r="272" spans="1:19">
@@ -17724,7 +17736,7 @@
         <v>1</v>
       </c>
       <c r="S272">
-        <v>1.5542E-05</v>
+        <v>3.8084E-05</v>
       </c>
     </row>
     <row r="273" spans="1:19">
@@ -17765,7 +17777,7 @@
         <v>0</v>
       </c>
       <c r="S273">
-        <v>2.1833E-05</v>
+        <v>0.000161333</v>
       </c>
     </row>
     <row r="274" spans="1:19">
@@ -17824,7 +17836,7 @@
         <v>2</v>
       </c>
       <c r="S274">
-        <v>1.1583E-05</v>
+        <v>6.179199999999999E-05</v>
       </c>
     </row>
     <row r="275" spans="1:19">
@@ -17871,7 +17883,7 @@
         <v>1</v>
       </c>
       <c r="S275">
-        <v>1.0709E-05</v>
+        <v>7.8625E-05</v>
       </c>
     </row>
     <row r="276" spans="1:19">
@@ -17912,7 +17924,7 @@
         <v>2</v>
       </c>
       <c r="S276">
-        <v>8.916999999999999E-06</v>
+        <v>7.4E-05</v>
       </c>
     </row>
     <row r="277" spans="1:19">
@@ -17959,7 +17971,7 @@
         <v>3</v>
       </c>
       <c r="S277">
-        <v>9.374999999999999E-06</v>
+        <v>1.7416E-05</v>
       </c>
     </row>
     <row r="278" spans="1:19">
@@ -17994,7 +18006,7 @@
         <v>1</v>
       </c>
       <c r="S278">
-        <v>9.125E-06</v>
+        <v>2.1458E-05</v>
       </c>
     </row>
     <row r="279" spans="1:19">
@@ -18035,7 +18047,7 @@
         <v>1</v>
       </c>
       <c r="S279">
-        <v>9.292E-06</v>
+        <v>2.1834E-05</v>
       </c>
     </row>
     <row r="280" spans="1:19">
@@ -18076,7 +18088,7 @@
         <v>2</v>
       </c>
       <c r="S280">
-        <v>7E-06</v>
+        <v>1.4708E-05</v>
       </c>
     </row>
     <row r="281" spans="1:19">
@@ -18129,7 +18141,7 @@
         <v>1</v>
       </c>
       <c r="S281">
-        <v>9.292E-06</v>
+        <v>2.4792E-05</v>
       </c>
     </row>
     <row r="282" spans="1:19">
@@ -18176,7 +18188,7 @@
         <v>3</v>
       </c>
       <c r="S282">
-        <v>9.167E-06</v>
+        <v>2.1E-05</v>
       </c>
     </row>
     <row r="283" spans="1:19">
@@ -18223,7 +18235,7 @@
         <v>3</v>
       </c>
       <c r="S283">
-        <v>6.166E-06</v>
+        <v>9.374999999999999E-06</v>
       </c>
     </row>
     <row r="284" spans="1:19">
@@ -18236,11 +18248,17 @@
       <c r="C284" t="s">
         <v>529</v>
       </c>
+      <c r="D284" t="s">
+        <v>529</v>
+      </c>
       <c r="E284" t="s">
         <v>529</v>
       </c>
+      <c r="F284" t="s">
+        <v>529</v>
+      </c>
       <c r="G284">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H284" t="s">
         <v>712</v>
@@ -18255,10 +18273,10 @@
         <v>1</v>
       </c>
       <c r="R284">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S284">
-        <v>8.291000000000001E-06</v>
+        <v>1.4375E-05</v>
       </c>
     </row>
     <row r="285" spans="1:19">
@@ -18317,7 +18335,7 @@
         <v>3</v>
       </c>
       <c r="S285">
-        <v>1.8833E-05</v>
+        <v>4.5334E-05</v>
       </c>
     </row>
     <row r="286" spans="1:19">
@@ -18364,7 +18382,7 @@
         <v>3</v>
       </c>
       <c r="S286">
-        <v>4.584E-06</v>
+        <v>7.666000000000001E-06</v>
       </c>
     </row>
     <row r="287" spans="1:19">
@@ -18399,7 +18417,7 @@
         <v>1</v>
       </c>
       <c r="S287">
-        <v>1.2875E-05</v>
+        <v>2.3333E-05</v>
       </c>
     </row>
     <row r="288" spans="1:19">
@@ -18440,7 +18458,7 @@
         <v>0</v>
       </c>
       <c r="S288">
-        <v>8E-06</v>
+        <v>1.375E-05</v>
       </c>
     </row>
     <row r="289" spans="1:19">
@@ -18481,7 +18499,7 @@
         <v>2</v>
       </c>
       <c r="S289">
-        <v>9.291E-06</v>
+        <v>1.5042E-05</v>
       </c>
     </row>
     <row r="290" spans="1:19">
@@ -18528,7 +18546,7 @@
         <v>3</v>
       </c>
       <c r="S290">
-        <v>7.083E-06</v>
+        <v>2.1834E-05</v>
       </c>
     </row>
     <row r="291" spans="1:19">
@@ -18581,7 +18599,7 @@
         <v>1</v>
       </c>
       <c r="S291">
-        <v>7.791E-06</v>
+        <v>1.6958E-05</v>
       </c>
     </row>
     <row r="292" spans="1:19">
@@ -18622,7 +18640,7 @@
         <v>2</v>
       </c>
       <c r="S292">
-        <v>9.208999999999999E-06</v>
+        <v>2E-05</v>
       </c>
     </row>
     <row r="293" spans="1:19">
@@ -18657,7 +18675,7 @@
         <v>1</v>
       </c>
       <c r="S293">
-        <v>6.625E-06</v>
+        <v>1.5833E-05</v>
       </c>
     </row>
     <row r="294" spans="1:19">
@@ -18710,7 +18728,7 @@
         <v>2</v>
       </c>
       <c r="S294">
-        <v>1.1041E-05</v>
+        <v>2.3291E-05</v>
       </c>
     </row>
     <row r="295" spans="1:19">
@@ -18745,7 +18763,7 @@
         <v>1</v>
       </c>
       <c r="S295">
-        <v>7.417E-06</v>
+        <v>1.85E-05</v>
       </c>
     </row>
     <row r="296" spans="1:19">
@@ -18780,7 +18798,7 @@
         <v>1</v>
       </c>
       <c r="S296">
-        <v>7.125E-06</v>
+        <v>8.208E-06</v>
       </c>
     </row>
     <row r="297" spans="1:19">
@@ -18827,7 +18845,7 @@
         <v>1</v>
       </c>
       <c r="S297">
-        <v>1.825E-05</v>
+        <v>3.8625E-05</v>
       </c>
     </row>
     <row r="298" spans="1:19">
@@ -18880,7 +18898,7 @@
         <v>1</v>
       </c>
       <c r="S298">
-        <v>1.2584E-05</v>
+        <v>2.7709E-05</v>
       </c>
     </row>
     <row r="299" spans="1:19">
@@ -18939,7 +18957,7 @@
         <v>3</v>
       </c>
       <c r="S299">
-        <v>1.2875E-05</v>
+        <v>2.6875E-05</v>
       </c>
     </row>
     <row r="300" spans="1:19">
@@ -18986,7 +19004,7 @@
         <v>3</v>
       </c>
       <c r="S300">
-        <v>5.917E-06</v>
+        <v>9.458E-06</v>
       </c>
     </row>
     <row r="301" spans="1:19">
@@ -19039,7 +19057,7 @@
         <v>2</v>
       </c>
       <c r="S301">
-        <v>1.5625E-05</v>
+        <v>4.5041E-05</v>
       </c>
     </row>
     <row r="302" spans="1:19">
@@ -19086,7 +19104,7 @@
         <v>3</v>
       </c>
       <c r="S302">
-        <v>8.165999999999999E-06</v>
+        <v>1.3541E-05</v>
       </c>
     </row>
     <row r="303" spans="1:19">
@@ -19133,7 +19151,7 @@
         <v>1</v>
       </c>
       <c r="S303">
-        <v>1.5667E-05</v>
+        <v>4.2E-05</v>
       </c>
     </row>
     <row r="304" spans="1:19">
@@ -19174,7 +19192,7 @@
         <v>2</v>
       </c>
       <c r="S304">
-        <v>5.208E-06</v>
+        <v>5.75E-06</v>
       </c>
     </row>
     <row r="305" spans="1:19">
@@ -19227,7 +19245,7 @@
         <v>2</v>
       </c>
       <c r="S305">
-        <v>1.0958E-05</v>
+        <v>1.475E-05</v>
       </c>
     </row>
     <row r="306" spans="1:19">
@@ -19268,7 +19286,7 @@
         <v>2</v>
       </c>
       <c r="S306">
-        <v>7.167E-06</v>
+        <v>1.2542E-05</v>
       </c>
     </row>
     <row r="307" spans="1:19">
@@ -19315,7 +19333,7 @@
         <v>3</v>
       </c>
       <c r="S307">
-        <v>1.0625E-05</v>
+        <v>1.5125E-05</v>
       </c>
     </row>
     <row r="308" spans="1:19">
@@ -19362,7 +19380,7 @@
         <v>3</v>
       </c>
       <c r="S308">
-        <v>7.791E-06</v>
+        <v>1.9791E-05</v>
       </c>
     </row>
     <row r="309" spans="1:19">
@@ -19421,7 +19439,7 @@
         <v>2</v>
       </c>
       <c r="S309">
-        <v>1.2834E-05</v>
+        <v>3.3584E-05</v>
       </c>
     </row>
     <row r="310" spans="1:19">
@@ -19468,7 +19486,7 @@
         <v>2</v>
       </c>
       <c r="S310">
-        <v>7.75E-06</v>
+        <v>1.85E-05</v>
       </c>
     </row>
     <row r="311" spans="1:19">
@@ -19527,7 +19545,7 @@
         <v>2</v>
       </c>
       <c r="S311">
-        <v>1.1625E-05</v>
+        <v>2.8042E-05</v>
       </c>
     </row>
     <row r="312" spans="1:19">
@@ -19568,7 +19586,7 @@
         <v>2</v>
       </c>
       <c r="S312">
-        <v>4.708E-06</v>
+        <v>7.458E-06</v>
       </c>
     </row>
     <row r="313" spans="1:19">
@@ -19609,7 +19627,7 @@
         <v>2</v>
       </c>
       <c r="S313">
-        <v>1.4417E-05</v>
+        <v>1.7042E-05</v>
       </c>
     </row>
     <row r="314" spans="1:19">
@@ -19650,7 +19668,7 @@
         <v>0</v>
       </c>
       <c r="S314">
-        <v>1.6292E-05</v>
+        <v>4.2333E-05</v>
       </c>
     </row>
     <row r="315" spans="1:19">
@@ -19691,7 +19709,7 @@
         <v>2</v>
       </c>
       <c r="S315">
-        <v>8E-06</v>
+        <v>1.2541E-05</v>
       </c>
     </row>
     <row r="316" spans="1:19">
@@ -19726,7 +19744,7 @@
         <v>1</v>
       </c>
       <c r="S316">
-        <v>7.832999999999999E-06</v>
+        <v>1.375E-05</v>
       </c>
     </row>
     <row r="317" spans="1:19">
@@ -19773,7 +19791,7 @@
         <v>3</v>
       </c>
       <c r="S317">
-        <v>9.541999999999999E-06</v>
+        <v>2.0875E-05</v>
       </c>
     </row>
     <row r="318" spans="1:19">
@@ -19820,7 +19838,7 @@
         <v>3</v>
       </c>
       <c r="S318">
-        <v>6.583E-06</v>
+        <v>1.1709E-05</v>
       </c>
     </row>
     <row r="319" spans="1:19">
@@ -19867,7 +19885,7 @@
         <v>3</v>
       </c>
       <c r="S319">
-        <v>9.374999999999999E-06</v>
+        <v>1.3625E-05</v>
       </c>
     </row>
     <row r="320" spans="1:19">
@@ -19920,7 +19938,7 @@
         <v>1</v>
       </c>
       <c r="S320">
-        <v>1.5833E-05</v>
+        <v>3.0625E-05</v>
       </c>
     </row>
     <row r="321" spans="1:19">
@@ -19967,7 +19985,7 @@
         <v>3</v>
       </c>
       <c r="S321">
-        <v>7.375E-06</v>
+        <v>1.4708E-05</v>
       </c>
     </row>
     <row r="322" spans="1:19">
@@ -20014,7 +20032,7 @@
         <v>1</v>
       </c>
       <c r="S322">
-        <v>1.1042E-05</v>
+        <v>2.0417E-05</v>
       </c>
     </row>
     <row r="323" spans="1:19">
@@ -20055,7 +20073,7 @@
         <v>2</v>
       </c>
       <c r="S323">
-        <v>8.833E-06</v>
+        <v>1.8208E-05</v>
       </c>
     </row>
     <row r="324" spans="1:19">
@@ -20090,7 +20108,7 @@
         <v>1</v>
       </c>
       <c r="S324">
-        <v>7.292E-06</v>
+        <v>1.3375E-05</v>
       </c>
     </row>
     <row r="325" spans="1:19">
@@ -20137,7 +20155,7 @@
         <v>2</v>
       </c>
       <c r="S325">
-        <v>9.625E-06</v>
+        <v>1.9166E-05</v>
       </c>
     </row>
     <row r="326" spans="1:19">
@@ -20190,7 +20208,7 @@
         <v>1</v>
       </c>
       <c r="S326">
-        <v>1.6E-05</v>
+        <v>3.2208E-05</v>
       </c>
     </row>
     <row r="327" spans="1:19">
@@ -20231,7 +20249,7 @@
         <v>2</v>
       </c>
       <c r="S327">
-        <v>9.959000000000001E-06</v>
+        <v>1.9666E-05</v>
       </c>
     </row>
     <row r="328" spans="1:19">
@@ -20278,7 +20296,7 @@
         <v>1</v>
       </c>
       <c r="S328">
-        <v>1.3834E-05</v>
+        <v>2.4916E-05</v>
       </c>
     </row>
     <row r="329" spans="1:19">
@@ -20291,11 +20309,17 @@
       <c r="C329" t="s">
         <v>484</v>
       </c>
+      <c r="D329" t="s">
+        <v>484</v>
+      </c>
       <c r="E329" t="s">
         <v>484</v>
       </c>
+      <c r="F329" t="s">
+        <v>484</v>
+      </c>
       <c r="G329">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H329" t="s">
         <v>729</v>
@@ -20316,10 +20340,10 @@
         <v>1</v>
       </c>
       <c r="R329">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S329">
-        <v>5.208E-06</v>
+        <v>6.959E-06</v>
       </c>
     </row>
     <row r="330" spans="1:19">
@@ -20366,7 +20390,7 @@
         <v>2</v>
       </c>
       <c r="S330">
-        <v>6.625E-06</v>
+        <v>8E-06</v>
       </c>
     </row>
     <row r="331" spans="1:19">
@@ -20413,7 +20437,7 @@
         <v>0</v>
       </c>
       <c r="S331">
-        <v>1.325E-05</v>
+        <v>2.0917E-05</v>
       </c>
     </row>
     <row r="332" spans="1:19">
@@ -20466,7 +20490,7 @@
         <v>1</v>
       </c>
       <c r="S332">
-        <v>2E-05</v>
+        <v>1.4834E-05</v>
       </c>
     </row>
     <row r="333" spans="1:19">
@@ -20513,7 +20537,7 @@
         <v>1</v>
       </c>
       <c r="S333">
-        <v>1.2792E-05</v>
+        <v>2.9875E-05</v>
       </c>
     </row>
     <row r="334" spans="1:19">
@@ -20554,7 +20578,7 @@
         <v>2</v>
       </c>
       <c r="S334">
-        <v>9.791E-06</v>
+        <v>1.5709E-05</v>
       </c>
     </row>
     <row r="335" spans="1:19">
@@ -20607,7 +20631,7 @@
         <v>2</v>
       </c>
       <c r="S335">
-        <v>1.2958E-05</v>
+        <v>2.1042E-05</v>
       </c>
     </row>
     <row r="336" spans="1:19">
@@ -20660,7 +20684,7 @@
         <v>2</v>
       </c>
       <c r="S336">
-        <v>6.416E-06</v>
+        <v>1.3416E-05</v>
       </c>
     </row>
     <row r="337" spans="1:19">
@@ -20719,7 +20743,7 @@
         <v>2</v>
       </c>
       <c r="S337">
-        <v>1.3917E-05</v>
+        <v>2.9875E-05</v>
       </c>
     </row>
     <row r="338" spans="1:19">
@@ -20772,7 +20796,7 @@
         <v>2</v>
       </c>
       <c r="S338">
-        <v>1.0458E-05</v>
+        <v>1.275E-05</v>
       </c>
     </row>
     <row r="339" spans="1:19">
@@ -20807,7 +20831,7 @@
         <v>1</v>
       </c>
       <c r="S339">
-        <v>9.25E-06</v>
+        <v>1.4958E-05</v>
       </c>
     </row>
     <row r="340" spans="1:19">
@@ -20854,7 +20878,7 @@
         <v>1</v>
       </c>
       <c r="S340">
-        <v>7.583E-06</v>
+        <v>1.5708E-05</v>
       </c>
     </row>
     <row r="341" spans="1:19">
@@ -20913,7 +20937,7 @@
         <v>2</v>
       </c>
       <c r="S341">
-        <v>8.875000000000001E-06</v>
+        <v>1.7584E-05</v>
       </c>
     </row>
     <row r="342" spans="1:19">
@@ -20960,7 +20984,7 @@
         <v>1</v>
       </c>
       <c r="S342">
-        <v>1.5375E-05</v>
+        <v>2.95E-05</v>
       </c>
     </row>
     <row r="343" spans="1:19">
@@ -21001,7 +21025,7 @@
         <v>2</v>
       </c>
       <c r="S343">
-        <v>5.292E-06</v>
+        <v>8.083E-06</v>
       </c>
     </row>
     <row r="344" spans="1:19">
@@ -21048,7 +21072,7 @@
         <v>3</v>
       </c>
       <c r="S344">
-        <v>1.1167E-05</v>
+        <v>1.1291E-05</v>
       </c>
     </row>
     <row r="345" spans="1:19">
@@ -21083,7 +21107,7 @@
         <v>1</v>
       </c>
       <c r="S345">
-        <v>9.167E-06</v>
+        <v>1.9375E-05</v>
       </c>
     </row>
     <row r="346" spans="1:19">
@@ -21183,7 +21207,7 @@
         <v>3</v>
       </c>
       <c r="S347">
-        <v>9.833000000000001E-06</v>
+        <v>1.3625E-05</v>
       </c>
     </row>
     <row r="348" spans="1:19">
@@ -21224,7 +21248,7 @@
         <v>2</v>
       </c>
       <c r="S348">
-        <v>7.042E-06</v>
+        <v>1.6959E-05</v>
       </c>
     </row>
     <row r="349" spans="1:19">
@@ -21277,7 +21301,7 @@
         <v>2</v>
       </c>
       <c r="S349">
-        <v>1.4042E-05</v>
+        <v>2.5125E-05</v>
       </c>
     </row>
     <row r="350" spans="1:19">
@@ -21318,7 +21342,7 @@
         <v>0</v>
       </c>
       <c r="S350">
-        <v>9.082999999999999E-06</v>
+        <v>1.6958E-05</v>
       </c>
     </row>
     <row r="351" spans="1:19">
@@ -21359,7 +21383,7 @@
         <v>0</v>
       </c>
       <c r="S351">
-        <v>1.6042E-05</v>
+        <v>2.8E-05</v>
       </c>
     </row>
     <row r="352" spans="1:19">
@@ -21400,7 +21424,7 @@
         <v>1</v>
       </c>
       <c r="S352">
-        <v>8.792E-06</v>
+        <v>1.8375E-05</v>
       </c>
     </row>
     <row r="353" spans="1:19">
@@ -21441,7 +21465,7 @@
         <v>0</v>
       </c>
       <c r="S353">
-        <v>9.500000000000001E-06</v>
+        <v>1.6875E-05</v>
       </c>
     </row>
     <row r="354" spans="1:19">
@@ -21482,7 +21506,7 @@
         <v>2</v>
       </c>
       <c r="S354">
-        <v>1.2541E-05</v>
+        <v>2.5334E-05</v>
       </c>
     </row>
     <row r="355" spans="1:19">
@@ -21529,7 +21553,7 @@
         <v>1</v>
       </c>
       <c r="S355">
-        <v>1.7875E-05</v>
+        <v>2.7458E-05</v>
       </c>
     </row>
     <row r="356" spans="1:19">
@@ -21570,7 +21594,7 @@
         <v>0</v>
       </c>
       <c r="S356">
-        <v>1.5625E-05</v>
+        <v>2.075E-05</v>
       </c>
     </row>
     <row r="357" spans="1:19">
@@ -21605,7 +21629,7 @@
         <v>1</v>
       </c>
       <c r="S357">
-        <v>6.958E-06</v>
+        <v>1.0916E-05</v>
       </c>
     </row>
     <row r="358" spans="1:19">
@@ -21646,7 +21670,7 @@
         <v>0</v>
       </c>
       <c r="S358">
-        <v>9.833000000000001E-06</v>
+        <v>1.5416E-05</v>
       </c>
     </row>
     <row r="359" spans="1:19">
@@ -21699,7 +21723,7 @@
         <v>2</v>
       </c>
       <c r="S359">
-        <v>9.500000000000001E-06</v>
+        <v>2.05E-05</v>
       </c>
     </row>
     <row r="360" spans="1:19">
@@ -21758,7 +21782,7 @@
         <v>2</v>
       </c>
       <c r="S360">
-        <v>1.5208E-05</v>
+        <v>3.3666E-05</v>
       </c>
     </row>
     <row r="361" spans="1:19">
@@ -21793,7 +21817,7 @@
         <v>1</v>
       </c>
       <c r="S361">
-        <v>7.584E-06</v>
+        <v>1.3792E-05</v>
       </c>
     </row>
     <row r="362" spans="1:19">
@@ -21828,7 +21852,7 @@
         <v>1</v>
       </c>
       <c r="S362">
-        <v>9.583E-06</v>
+        <v>1.5709E-05</v>
       </c>
     </row>
     <row r="363" spans="1:19">
@@ -21881,7 +21905,7 @@
         <v>2</v>
       </c>
       <c r="S363">
-        <v>7.041E-06</v>
+        <v>1.1334E-05</v>
       </c>
     </row>
     <row r="364" spans="1:19">
@@ -21922,7 +21946,7 @@
         <v>0</v>
       </c>
       <c r="S364">
-        <v>2.0084E-05</v>
+        <v>3.4666E-05</v>
       </c>
     </row>
     <row r="365" spans="1:19">
@@ -21957,7 +21981,7 @@
         <v>1</v>
       </c>
       <c r="S365">
-        <v>5.792E-06</v>
+        <v>7.5E-06</v>
       </c>
     </row>
     <row r="366" spans="1:19">
@@ -22004,7 +22028,7 @@
         <v>3</v>
       </c>
       <c r="S366">
-        <v>4.084E-06</v>
+        <v>5.916E-06</v>
       </c>
     </row>
     <row r="367" spans="1:19">
@@ -22051,7 +22075,7 @@
         <v>1</v>
       </c>
       <c r="S367">
-        <v>1.4667E-05</v>
+        <v>1.8917E-05</v>
       </c>
     </row>
     <row r="368" spans="1:19">
@@ -22104,7 +22128,7 @@
         <v>2</v>
       </c>
       <c r="S368">
-        <v>1.5416E-05</v>
+        <v>2.3292E-05</v>
       </c>
     </row>
     <row r="369" spans="1:19">
@@ -22145,7 +22169,7 @@
         <v>0</v>
       </c>
       <c r="S369">
-        <v>1.3125E-05</v>
+        <v>3.0584E-05</v>
       </c>
     </row>
     <row r="370" spans="1:19">
@@ -22186,7 +22210,7 @@
         <v>2</v>
       </c>
       <c r="S370">
-        <v>6.25E-06</v>
+        <v>1.3292E-05</v>
       </c>
     </row>
     <row r="371" spans="1:19">
@@ -22227,7 +22251,7 @@
         <v>2</v>
       </c>
       <c r="S371">
-        <v>1.1958E-05</v>
+        <v>2.5709E-05</v>
       </c>
     </row>
     <row r="372" spans="1:19">
@@ -22280,7 +22304,7 @@
         <v>1</v>
       </c>
       <c r="S372">
-        <v>1.0834E-05</v>
+        <v>2.1959E-05</v>
       </c>
     </row>
     <row r="373" spans="1:19">
@@ -22327,7 +22351,7 @@
         <v>1</v>
       </c>
       <c r="S373">
-        <v>1.0875E-05</v>
+        <v>1.6167E-05</v>
       </c>
     </row>
     <row r="374" spans="1:19">
@@ -22368,7 +22392,7 @@
         <v>0</v>
       </c>
       <c r="S374">
-        <v>9.042000000000001E-06</v>
+        <v>0.000137041</v>
       </c>
     </row>
     <row r="375" spans="1:19">
@@ -22415,7 +22439,7 @@
         <v>1</v>
       </c>
       <c r="S375">
-        <v>8.749999999999999E-06</v>
+        <v>6.2791E-05</v>
       </c>
     </row>
     <row r="376" spans="1:19">
@@ -22462,7 +22486,7 @@
         <v>1</v>
       </c>
       <c r="S376">
-        <v>1.3166E-05</v>
+        <v>6.6208E-05</v>
       </c>
     </row>
     <row r="377" spans="1:19">
@@ -22503,7 +22527,7 @@
         <v>2</v>
       </c>
       <c r="S377">
-        <v>9.458E-06</v>
+        <v>2.3125E-05</v>
       </c>
     </row>
     <row r="378" spans="1:19">
@@ -22538,7 +22562,7 @@
         <v>1</v>
       </c>
       <c r="S378">
-        <v>7.541E-06</v>
+        <v>1.5708E-05</v>
       </c>
     </row>
     <row r="379" spans="1:19">
@@ -22579,7 +22603,7 @@
         <v>2</v>
       </c>
       <c r="S379">
-        <v>6.625E-06</v>
+        <v>1.4125E-05</v>
       </c>
     </row>
     <row r="380" spans="1:19">
@@ -22632,7 +22656,7 @@
         <v>2</v>
       </c>
       <c r="S380">
-        <v>1.2667E-05</v>
+        <v>3.1041E-05</v>
       </c>
     </row>
     <row r="381" spans="1:19">
@@ -22685,7 +22709,7 @@
         <v>1</v>
       </c>
       <c r="S381">
-        <v>1.2041E-05</v>
+        <v>2.1459E-05</v>
       </c>
     </row>
     <row r="382" spans="1:19">
@@ -22732,7 +22756,7 @@
         <v>1</v>
       </c>
       <c r="S382">
-        <v>7.832999999999999E-06</v>
+        <v>1.8708E-05</v>
       </c>
     </row>
     <row r="383" spans="1:19">
@@ -22785,7 +22809,7 @@
         <v>1</v>
       </c>
       <c r="S383">
-        <v>1.3834E-05</v>
+        <v>2.55E-05</v>
       </c>
     </row>
     <row r="384" spans="1:19">
@@ -22838,7 +22862,7 @@
         <v>1</v>
       </c>
       <c r="S384">
-        <v>1.2292E-05</v>
+        <v>2.5083E-05</v>
       </c>
     </row>
     <row r="385" spans="1:19">
@@ -22873,7 +22897,7 @@
         <v>1</v>
       </c>
       <c r="S385">
-        <v>1.1375E-05</v>
+        <v>1.675E-05</v>
       </c>
     </row>
     <row r="386" spans="1:19">
@@ -22932,7 +22956,7 @@
         <v>2</v>
       </c>
       <c r="S386">
-        <v>9.707999999999999E-06</v>
+        <v>1.1625E-05</v>
       </c>
     </row>
     <row r="387" spans="1:19">
@@ -22973,7 +22997,7 @@
         <v>2</v>
       </c>
       <c r="S387">
-        <v>1.2666E-05</v>
+        <v>3.6125E-05</v>
       </c>
     </row>
     <row r="388" spans="1:19">
@@ -23026,7 +23050,7 @@
         <v>2</v>
       </c>
       <c r="S388">
-        <v>1.2958E-05</v>
+        <v>3.7459E-05</v>
       </c>
     </row>
     <row r="389" spans="1:19">
@@ -23085,7 +23109,7 @@
         <v>3</v>
       </c>
       <c r="S389">
-        <v>1.2792E-05</v>
+        <v>3.3583E-05</v>
       </c>
     </row>
     <row r="390" spans="1:19">
@@ -23144,7 +23168,7 @@
         <v>1</v>
       </c>
       <c r="S390">
-        <v>8.292E-06</v>
+        <v>2.5125E-05</v>
       </c>
     </row>
     <row r="391" spans="1:19">
@@ -23185,7 +23209,7 @@
         <v>0</v>
       </c>
       <c r="S391">
-        <v>1.4625E-05</v>
+        <v>2.0625E-05</v>
       </c>
     </row>
     <row r="392" spans="1:19">
@@ -23244,7 +23268,7 @@
         <v>3</v>
       </c>
       <c r="S392">
-        <v>8.834E-06</v>
+        <v>1.5334E-05</v>
       </c>
     </row>
     <row r="393" spans="1:19">
@@ -23291,7 +23315,7 @@
         <v>1</v>
       </c>
       <c r="S393">
-        <v>1.8208E-05</v>
+        <v>5.1542E-05</v>
       </c>
     </row>
     <row r="394" spans="1:19">
@@ -23344,7 +23368,7 @@
         <v>2</v>
       </c>
       <c r="S394">
-        <v>1.1583E-05</v>
+        <v>2.5584E-05</v>
       </c>
     </row>
     <row r="395" spans="1:19">
@@ -23379,7 +23403,7 @@
         <v>1</v>
       </c>
       <c r="S395">
-        <v>4.958E-06</v>
+        <v>3.6166E-05</v>
       </c>
     </row>
     <row r="396" spans="1:19">
@@ -23426,7 +23450,7 @@
         <v>1</v>
       </c>
       <c r="S396">
-        <v>1.5375E-05</v>
+        <v>2.7709E-05</v>
       </c>
     </row>
     <row r="397" spans="1:19">
@@ -23473,7 +23497,7 @@
         <v>3</v>
       </c>
       <c r="S397">
-        <v>7.042E-06</v>
+        <v>1.5917E-05</v>
       </c>
     </row>
     <row r="398" spans="1:19">
@@ -23514,7 +23538,7 @@
         <v>2</v>
       </c>
       <c r="S398">
-        <v>5.5E-06</v>
+        <v>6.417E-06</v>
       </c>
     </row>
     <row r="399" spans="1:19">
@@ -23561,7 +23585,7 @@
         <v>1</v>
       </c>
       <c r="S399">
-        <v>1.5542E-05</v>
+        <v>3.8166E-05</v>
       </c>
     </row>
     <row r="400" spans="1:19">
@@ -23608,7 +23632,7 @@
         <v>3</v>
       </c>
       <c r="S400">
-        <v>4.042E-06</v>
+        <v>6.417E-06</v>
       </c>
     </row>
     <row r="401" spans="1:19">
@@ -23661,7 +23685,7 @@
         <v>2</v>
       </c>
       <c r="S401">
-        <v>1.7125E-05</v>
+        <v>3.1542E-05</v>
       </c>
     </row>
     <row r="402" spans="1:19">
@@ -23702,7 +23726,7 @@
         <v>2</v>
       </c>
       <c r="S402">
-        <v>1.2084E-05</v>
+        <v>3.6625E-05</v>
       </c>
     </row>
     <row r="403" spans="1:19">
@@ -23749,7 +23773,7 @@
         <v>3</v>
       </c>
       <c r="S403">
-        <v>8.416999999999999E-06</v>
+        <v>1.7625E-05</v>
       </c>
     </row>
     <row r="404" spans="1:19">
@@ -23796,7 +23820,7 @@
         <v>3</v>
       </c>
       <c r="S404">
-        <v>1.0041E-05</v>
+        <v>4.5542E-05</v>
       </c>
     </row>
     <row r="405" spans="1:19">
@@ -23837,7 +23861,7 @@
         <v>2</v>
       </c>
       <c r="S405">
-        <v>9.167E-06</v>
+        <v>0.000161834</v>
       </c>
     </row>
     <row r="406" spans="1:19">
@@ -23890,7 +23914,7 @@
         <v>2</v>
       </c>
       <c r="S406">
-        <v>1.8041E-05</v>
+        <v>2.9833E-05</v>
       </c>
     </row>
     <row r="407" spans="1:19">
@@ -23937,7 +23961,7 @@
         <v>3</v>
       </c>
       <c r="S407">
-        <v>1.0875E-05</v>
+        <v>1.5708E-05</v>
       </c>
     </row>
     <row r="408" spans="1:19">
@@ -23984,7 +24008,7 @@
         <v>1</v>
       </c>
       <c r="S408">
-        <v>1.3291E-05</v>
+        <v>2.3917E-05</v>
       </c>
     </row>
     <row r="409" spans="1:19">
@@ -24031,7 +24055,7 @@
         <v>3</v>
       </c>
       <c r="S409">
-        <v>5.666E-06</v>
+        <v>9.584E-06</v>
       </c>
     </row>
     <row r="410" spans="1:19">
@@ -24078,7 +24102,7 @@
         <v>3</v>
       </c>
       <c r="S410">
-        <v>9.917E-06</v>
+        <v>2.9125E-05</v>
       </c>
     </row>
     <row r="411" spans="1:19">
@@ -24131,7 +24155,7 @@
         <v>2</v>
       </c>
       <c r="S411">
-        <v>8.375E-06</v>
+        <v>2.4667E-05</v>
       </c>
     </row>
     <row r="412" spans="1:19">
@@ -24190,7 +24214,7 @@
         <v>3</v>
       </c>
       <c r="S412">
-        <v>1.2084E-05</v>
+        <v>3.0375E-05</v>
       </c>
     </row>
     <row r="413" spans="1:19">
@@ -24231,7 +24255,7 @@
         <v>2</v>
       </c>
       <c r="S413">
-        <v>1.0292E-05</v>
+        <v>3.4833E-05</v>
       </c>
     </row>
     <row r="414" spans="1:19">
@@ -24284,7 +24308,7 @@
         <v>2</v>
       </c>
       <c r="S414">
-        <v>1.1125E-05</v>
+        <v>4.4792E-05</v>
       </c>
     </row>
     <row r="415" spans="1:19">
@@ -24337,7 +24361,7 @@
         <v>2</v>
       </c>
       <c r="S415">
-        <v>6E-06</v>
+        <v>1.5E-05</v>
       </c>
     </row>
     <row r="416" spans="1:19">
@@ -24396,7 +24420,7 @@
         <v>3</v>
       </c>
       <c r="S416">
-        <v>8.666E-06</v>
+        <v>2.1042E-05</v>
       </c>
     </row>
     <row r="417" spans="1:19">
@@ -24443,7 +24467,7 @@
         <v>2</v>
       </c>
       <c r="S417">
-        <v>6.0375E-05</v>
+        <v>1.3417E-05</v>
       </c>
     </row>
     <row r="418" spans="1:19">
@@ -24478,7 +24502,7 @@
         <v>1</v>
       </c>
       <c r="S418">
-        <v>7.662500000000001E-05</v>
+        <v>1.6666E-05</v>
       </c>
     </row>
     <row r="419" spans="1:19">
@@ -24531,7 +24555,7 @@
         <v>2</v>
       </c>
       <c r="S419">
-        <v>1.0292E-05</v>
+        <v>1.7834E-05</v>
       </c>
     </row>
     <row r="420" spans="1:19">
@@ -24572,7 +24596,7 @@
         <v>2</v>
       </c>
       <c r="S420">
-        <v>7.333E-06</v>
+        <v>1.3208E-05</v>
       </c>
     </row>
     <row r="421" spans="1:19">
@@ -24625,7 +24649,7 @@
         <v>2</v>
       </c>
       <c r="S421">
-        <v>1.2792E-05</v>
+        <v>2.775E-05</v>
       </c>
     </row>
     <row r="422" spans="1:19">
@@ -24672,7 +24696,7 @@
         <v>1</v>
       </c>
       <c r="S422">
-        <v>2.4958E-05</v>
+        <v>2.7958E-05</v>
       </c>
     </row>
     <row r="423" spans="1:19">
@@ -24713,7 +24737,7 @@
         <v>2</v>
       </c>
       <c r="S423">
-        <v>1.2208E-05</v>
+        <v>1.6E-05</v>
       </c>
     </row>
     <row r="424" spans="1:19">
@@ -24760,7 +24784,7 @@
         <v>1</v>
       </c>
       <c r="S424">
-        <v>1.8333E-05</v>
+        <v>3.0791E-05</v>
       </c>
     </row>
     <row r="425" spans="1:19">
@@ -24807,7 +24831,7 @@
         <v>0</v>
       </c>
       <c r="S425">
-        <v>2.675E-05</v>
+        <v>3.45E-05</v>
       </c>
     </row>
     <row r="426" spans="1:19">
@@ -24860,7 +24884,7 @@
         <v>2</v>
       </c>
       <c r="S426">
-        <v>1.7584E-05</v>
+        <v>2.9875E-05</v>
       </c>
     </row>
     <row r="427" spans="1:19">
@@ -24913,7 +24937,7 @@
         <v>1</v>
       </c>
       <c r="S427">
-        <v>1.9833E-05</v>
+        <v>3.0208E-05</v>
       </c>
     </row>
     <row r="428" spans="1:19">
@@ -24966,7 +24990,7 @@
         <v>1</v>
       </c>
       <c r="S428">
-        <v>1.7958E-05</v>
+        <v>2.5125E-05</v>
       </c>
     </row>
     <row r="429" spans="1:19">
@@ -25001,7 +25025,7 @@
         <v>1</v>
       </c>
       <c r="S429">
-        <v>1E-05</v>
+        <v>1.6875E-05</v>
       </c>
     </row>
     <row r="430" spans="1:19">
@@ -25048,7 +25072,7 @@
         <v>1</v>
       </c>
       <c r="S430">
-        <v>2.9958E-05</v>
+        <v>4.675E-05</v>
       </c>
     </row>
     <row r="431" spans="1:19">
@@ -25095,7 +25119,7 @@
         <v>1</v>
       </c>
       <c r="S431">
-        <v>9.0042E-05</v>
+        <v>4.6084E-05</v>
       </c>
     </row>
     <row r="432" spans="1:19">
@@ -25154,7 +25178,7 @@
         <v>2</v>
       </c>
       <c r="S432">
-        <v>4.9333E-05</v>
+        <v>2.9958E-05</v>
       </c>
     </row>
     <row r="433" spans="1:19">
@@ -25207,7 +25231,7 @@
         <v>2</v>
       </c>
       <c r="S433">
-        <v>8.334E-06</v>
+        <v>7.334E-06</v>
       </c>
     </row>
     <row r="434" spans="1:19">
@@ -25242,7 +25266,7 @@
         <v>1</v>
       </c>
       <c r="S434">
-        <v>2.85E-05</v>
+        <v>2.5125E-05</v>
       </c>
     </row>
     <row r="435" spans="1:19">
@@ -25277,7 +25301,7 @@
         <v>1</v>
       </c>
       <c r="S435">
-        <v>1.5291E-05</v>
+        <v>3.4166E-05</v>
       </c>
     </row>
     <row r="436" spans="1:19">
@@ -25318,7 +25342,7 @@
         <v>2</v>
       </c>
       <c r="S436">
-        <v>1.3959E-05</v>
+        <v>2.9417E-05</v>
       </c>
     </row>
     <row r="437" spans="1:19">
@@ -25365,7 +25389,7 @@
         <v>3</v>
       </c>
       <c r="S437">
-        <v>7E-06</v>
+        <v>8.208E-06</v>
       </c>
     </row>
     <row r="438" spans="1:19">
@@ -25406,7 +25430,7 @@
         <v>2</v>
       </c>
       <c r="S438">
-        <v>8.124999999999999E-06</v>
+        <v>8.875000000000001E-06</v>
       </c>
     </row>
     <row r="439" spans="1:19">
@@ -25441,7 +25465,7 @@
         <v>1</v>
       </c>
       <c r="S439">
-        <v>1.2333E-05</v>
+        <v>2.5333E-05</v>
       </c>
     </row>
     <row r="440" spans="1:19">
@@ -25494,7 +25518,7 @@
         <v>1</v>
       </c>
       <c r="S440">
-        <v>2.3542E-05</v>
+        <v>3.5125E-05</v>
       </c>
     </row>
     <row r="441" spans="1:19">
@@ -25547,7 +25571,7 @@
         <v>2</v>
       </c>
       <c r="S441">
-        <v>1.6708E-05</v>
+        <v>1.425E-05</v>
       </c>
     </row>
     <row r="442" spans="1:19">
@@ -25569,11 +25593,17 @@
       <c r="H442" t="s">
         <v>791</v>
       </c>
+      <c r="I442" t="s">
+        <v>791</v>
+      </c>
       <c r="J442" t="s">
         <v>791</v>
       </c>
+      <c r="K442" t="s">
+        <v>791</v>
+      </c>
       <c r="L442">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M442" t="s">
         <v>1130</v>
@@ -25591,10 +25621,10 @@
         <v>1</v>
       </c>
       <c r="R442">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S442">
-        <v>1.4E-05</v>
+        <v>2.1167E-05</v>
       </c>
     </row>
     <row r="443" spans="1:19">
@@ -25635,7 +25665,7 @@
         <v>2</v>
       </c>
       <c r="S443">
-        <v>1.35E-05</v>
+        <v>2.9583E-05</v>
       </c>
     </row>
     <row r="444" spans="1:19">
@@ -25688,7 +25718,7 @@
         <v>2</v>
       </c>
       <c r="S444">
-        <v>2.3125E-05</v>
+        <v>2.8875E-05</v>
       </c>
     </row>
     <row r="445" spans="1:19">
@@ -25729,7 +25759,7 @@
         <v>0</v>
       </c>
       <c r="S445">
-        <v>2.1125E-05</v>
+        <v>2.675E-05</v>
       </c>
     </row>
     <row r="446" spans="1:19">
@@ -25788,7 +25818,7 @@
         <v>3</v>
       </c>
       <c r="S446">
-        <v>2.0833E-05</v>
+        <v>3.5458E-05</v>
       </c>
     </row>
     <row r="447" spans="1:19">
@@ -25835,7 +25865,7 @@
         <v>2</v>
       </c>
       <c r="S447">
-        <v>8.749999999999999E-06</v>
+        <v>6.308300000000001E-05</v>
       </c>
     </row>
     <row r="448" spans="1:19">
@@ -25882,7 +25912,7 @@
         <v>2</v>
       </c>
       <c r="S448">
-        <v>1.2625E-05</v>
+        <v>2.55E-05</v>
       </c>
     </row>
     <row r="449" spans="1:19">
@@ -25917,7 +25947,7 @@
         <v>1</v>
       </c>
       <c r="S449">
-        <v>6.334E-06</v>
+        <v>8.916000000000001E-06</v>
       </c>
     </row>
     <row r="450" spans="1:19">
@@ -25970,7 +26000,7 @@
         <v>1</v>
       </c>
       <c r="S450">
-        <v>1.4583E-05</v>
+        <v>2.3375E-05</v>
       </c>
     </row>
     <row r="451" spans="1:19">
@@ -26023,7 +26053,7 @@
         <v>2</v>
       </c>
       <c r="S451">
-        <v>1.9542E-05</v>
+        <v>5.0375E-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>